<commit_message>
Another new organization for background information
</commit_message>
<xml_diff>
--- a/tncData.xlsx
+++ b/tncData.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="tncData" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
   <si>
     <t>.wav file</t>
   </si>
@@ -106,6 +106,36 @@
   </si>
   <si>
     <t>Kam Plus</t>
+  </si>
+  <si>
+    <t>PK-232MBX</t>
+  </si>
+  <si>
+    <t>Kam</t>
+  </si>
+  <si>
+    <t>My Kam Plus</t>
+  </si>
+  <si>
+    <t>My PK-88</t>
+  </si>
+  <si>
+    <t>MFJ-1278</t>
+  </si>
+  <si>
+    <t>Goertzel PreClocking</t>
+  </si>
+  <si>
+    <t>Goertzel Max Preclocking</t>
+  </si>
+  <si>
+    <t>PLL</t>
+  </si>
+  <si>
+    <t>Goertzel Optimized window</t>
+  </si>
+  <si>
+    <t>Threaded Goertzel</t>
   </si>
 </sst>
 </file>
@@ -1025,20 +1055,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X19"/>
+  <dimension ref="A1:AH19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="U18" sqref="U18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.140625" customWidth="1"/>
     <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="24" width="11.5703125" customWidth="1"/>
+    <col min="3" max="34" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1064,47 +1094,77 @@
         <v>13</v>
       </c>
       <c r="I1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="P1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="S1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="T1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="V1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="W1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="Z1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="AA1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1" t="s">
+      <c r="AF1" s="1"/>
+      <c r="AG1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
@@ -1130,48 +1190,76 @@
         <v>40</v>
       </c>
       <c r="I2" s="4">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="J2" s="4">
-        <v>40</v>
-      </c>
-      <c r="K2" s="10">
+        <v>0</v>
+      </c>
+      <c r="K2" s="4">
         <v>40</v>
       </c>
       <c r="L2" s="4">
         <v>40</v>
       </c>
-      <c r="M2" s="4">
+      <c r="M2" s="4"/>
+      <c r="N2" s="4">
+        <v>40</v>
+      </c>
+      <c r="O2" s="4">
+        <v>40</v>
+      </c>
+      <c r="P2" s="10">
+        <v>40</v>
+      </c>
+      <c r="Q2" s="4">
+        <v>40</v>
+      </c>
+      <c r="R2" s="4">
         <v>39</v>
       </c>
-      <c r="N2" s="6">
-        <v>40</v>
-      </c>
-      <c r="O2" s="4">
-        <v>40</v>
-      </c>
-      <c r="P2" s="4">
-        <v>40</v>
-      </c>
-      <c r="Q2" s="6">
-        <v>40</v>
-      </c>
-      <c r="R2" s="4">
-        <v>40</v>
-      </c>
-      <c r="S2" s="4">
-        <v>40</v>
-      </c>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1">
-        <f>MAX(C2:V2)</f>
-        <v>40</v>
-      </c>
-      <c r="X2" s="1">
+      <c r="S2" s="6">
+        <v>40</v>
+      </c>
+      <c r="T2" s="4">
+        <v>40</v>
+      </c>
+      <c r="U2" s="4">
+        <v>40</v>
+      </c>
+      <c r="V2" s="4">
+        <v>40</v>
+      </c>
+      <c r="W2" s="4">
+        <v>40</v>
+      </c>
+      <c r="X2" s="4">
+        <v>40</v>
+      </c>
+      <c r="Y2" s="4">
+        <v>40</v>
+      </c>
+      <c r="Z2" s="4">
+        <v>40</v>
+      </c>
+      <c r="AA2" s="6">
+        <v>40</v>
+      </c>
+      <c r="AB2" s="4">
+        <v>40</v>
+      </c>
+      <c r="AC2" s="4">
+        <v>40</v>
+      </c>
+      <c r="AF2" s="1"/>
+      <c r="AG2" s="1">
+        <f>MAX(C2:AF2)</f>
+        <v>40</v>
+      </c>
+      <c r="AH2" s="1">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="5" t="s">
         <v>24</v>
@@ -1195,28 +1283,46 @@
         <v>40</v>
       </c>
       <c r="I3" s="5">
-        <v>0</v>
-      </c>
-      <c r="J3" s="5"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="5"/>
+        <v>40</v>
+      </c>
+      <c r="J3" s="5">
+        <v>0</v>
+      </c>
+      <c r="K3" s="5">
+        <v>40</v>
+      </c>
+      <c r="L3" s="5">
+        <v>40</v>
+      </c>
       <c r="M3" s="5"/>
-      <c r="N3" s="7"/>
+      <c r="N3" s="5">
+        <v>40</v>
+      </c>
       <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="7"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="5"/>
       <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1">
-        <f t="shared" ref="W3:W14" si="0">MAX(C3:V3)</f>
-        <v>40</v>
-      </c>
-      <c r="X3" s="1">
+      <c r="S3" s="7"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
+      <c r="W3" s="5"/>
+      <c r="X3" s="5"/>
+      <c r="Y3" s="5"/>
+      <c r="Z3" s="5"/>
+      <c r="AA3" s="7"/>
+      <c r="AB3" s="5"/>
+      <c r="AC3" s="5"/>
+      <c r="AF3" s="1"/>
+      <c r="AG3" s="1">
+        <f t="shared" ref="AG3:AG14" si="0">MAX(C3:AF3)</f>
+        <v>40</v>
+      </c>
+      <c r="AH3" s="1">
         <v>184</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
         <v>25</v>
@@ -1240,28 +1346,46 @@
         <v>40</v>
       </c>
       <c r="I4" s="3">
-        <v>0</v>
-      </c>
-      <c r="J4" s="3"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="3"/>
+        <v>40</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0</v>
+      </c>
+      <c r="K4" s="3">
+        <v>40</v>
+      </c>
+      <c r="L4" s="3">
+        <v>40</v>
+      </c>
       <c r="M4" s="3"/>
-      <c r="N4" s="8"/>
+      <c r="N4" s="3">
+        <v>0</v>
+      </c>
       <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="8"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="3"/>
       <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="V4" s="1"/>
-      <c r="W4" s="1">
+      <c r="S4" s="8"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="8"/>
+      <c r="AB4" s="3"/>
+      <c r="AC4" s="3"/>
+      <c r="AF4" s="1"/>
+      <c r="AG4" s="1">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="X4" s="1">
+      <c r="AH4" s="1">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -1287,46 +1411,74 @@
         <v>200</v>
       </c>
       <c r="I5" s="1">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="J5" s="1">
-        <v>200</v>
-      </c>
-      <c r="K5" s="11">
-        <v>200</v>
-      </c>
-      <c r="L5" s="5">
-        <v>200</v>
-      </c>
-      <c r="M5" s="5">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1">
+        <v>200</v>
+      </c>
+      <c r="L5" s="1">
+        <v>200</v>
+      </c>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1">
+        <v>200</v>
+      </c>
+      <c r="O5" s="1">
+        <v>200</v>
+      </c>
+      <c r="P5" s="11">
+        <v>200</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>200</v>
+      </c>
+      <c r="R5" s="5">
         <v>193</v>
       </c>
-      <c r="N5" s="7">
+      <c r="S5" s="7">
         <v>199</v>
       </c>
-      <c r="O5" s="1">
-        <v>200</v>
-      </c>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="7">
-        <v>200</v>
-      </c>
-      <c r="R5" s="1">
-        <v>200</v>
-      </c>
-      <c r="S5" s="1">
-        <v>200</v>
-      </c>
-      <c r="V5" s="1"/>
+      <c r="T5" s="5">
+        <v>200</v>
+      </c>
+      <c r="U5" s="5">
+        <v>200</v>
+      </c>
+      <c r="V5" s="1">
+        <v>200</v>
+      </c>
       <c r="W5" s="1">
+        <v>200</v>
+      </c>
+      <c r="X5" s="1">
+        <v>200</v>
+      </c>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1">
+        <v>200</v>
+      </c>
+      <c r="AA5" s="7">
+        <v>200</v>
+      </c>
+      <c r="AB5" s="1">
+        <v>200</v>
+      </c>
+      <c r="AC5" s="1">
+        <v>200</v>
+      </c>
+      <c r="AF5" s="1"/>
+      <c r="AG5" s="1">
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
-      <c r="X5" s="1">
+      <c r="AH5" s="1">
         <v>1549</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="5" t="s">
         <v>24</v>
@@ -1350,28 +1502,46 @@
         <v>200</v>
       </c>
       <c r="I6" s="1">
-        <v>0</v>
-      </c>
-      <c r="J6" s="1"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="7"/>
+        <v>200</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1">
+        <v>200</v>
+      </c>
+      <c r="L6" s="1">
+        <v>200</v>
+      </c>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1">
+        <v>200</v>
+      </c>
       <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
       <c r="V6" s="1"/>
-      <c r="W6" s="1">
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="7"/>
+      <c r="AB6" s="1"/>
+      <c r="AC6" s="1"/>
+      <c r="AF6" s="1"/>
+      <c r="AG6" s="1">
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
-      <c r="X6" s="1">
+      <c r="AH6" s="1">
         <v>1549</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3" t="s">
         <v>25</v>
@@ -1395,28 +1565,46 @@
         <v>200</v>
       </c>
       <c r="I7" s="3">
-        <v>0</v>
-      </c>
-      <c r="J7" s="3"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="3"/>
+        <v>200</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0</v>
+      </c>
+      <c r="K7" s="3">
+        <v>200</v>
+      </c>
+      <c r="L7" s="3">
+        <v>200</v>
+      </c>
       <c r="M7" s="3"/>
-      <c r="N7" s="8"/>
+      <c r="N7" s="3">
+        <v>200</v>
+      </c>
       <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="8"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
-      <c r="S7" s="3"/>
-      <c r="V7" s="1"/>
-      <c r="W7" s="1">
+      <c r="S7" s="8"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="8"/>
+      <c r="AB7" s="3"/>
+      <c r="AC7" s="3"/>
+      <c r="AF7" s="1"/>
+      <c r="AG7" s="1">
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
-      <c r="X7" s="2">
+      <c r="AH7" s="2">
         <v>2.3069444444444445</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
@@ -1442,46 +1630,74 @@
         <v>17</v>
       </c>
       <c r="I8" s="1">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="J8" s="1">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1">
+        <v>27</v>
+      </c>
+      <c r="L8" s="1">
+        <v>27</v>
+      </c>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1">
         <v>21</v>
       </c>
-      <c r="K8" s="11">
+      <c r="O8" s="1">
+        <v>21</v>
+      </c>
+      <c r="P8" s="11">
         <v>5</v>
       </c>
-      <c r="L8" s="5">
+      <c r="Q8" s="5">
         <v>16</v>
       </c>
-      <c r="M8" s="5">
+      <c r="R8" s="5">
         <v>13</v>
       </c>
-      <c r="N8" s="7">
+      <c r="S8" s="7">
         <v>12</v>
       </c>
-      <c r="O8" s="1">
+      <c r="T8" s="5">
+        <v>20</v>
+      </c>
+      <c r="U8" s="5">
         <v>12</v>
       </c>
-      <c r="P8" s="1">
+      <c r="V8" s="1">
+        <v>12</v>
+      </c>
+      <c r="W8" s="1">
+        <v>5</v>
+      </c>
+      <c r="X8" s="1">
         <v>25</v>
       </c>
-      <c r="Q8" s="7">
+      <c r="Y8" s="1">
+        <v>25</v>
+      </c>
+      <c r="Z8" s="1">
+        <v>12</v>
+      </c>
+      <c r="AA8" s="7">
         <v>18</v>
       </c>
-      <c r="R8" s="1">
+      <c r="AB8" s="1">
         <v>24</v>
       </c>
-      <c r="S8" s="1">
+      <c r="AC8" s="1">
         <v>24</v>
       </c>
-      <c r="V8" s="1"/>
-      <c r="W8" s="1">
+      <c r="AF8" s="1"/>
+      <c r="AG8" s="1">
         <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="X8" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="AH8" s="1"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="5" t="s">
         <v>24</v>
@@ -1505,26 +1721,44 @@
         <v>21</v>
       </c>
       <c r="I9" s="1">
-        <v>0</v>
-      </c>
-      <c r="J9" s="1"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="7"/>
+        <v>23</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1">
+        <v>26</v>
+      </c>
+      <c r="L9" s="1">
+        <v>26</v>
+      </c>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1">
+        <v>23</v>
+      </c>
       <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="1"/>
-      <c r="S9" s="1"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
       <c r="V9" s="1"/>
-      <c r="W9" s="1">
+      <c r="W9" s="1"/>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="1"/>
+      <c r="Z9" s="1"/>
+      <c r="AA9" s="7"/>
+      <c r="AB9" s="1"/>
+      <c r="AC9" s="1"/>
+      <c r="AF9" s="1"/>
+      <c r="AG9" s="1">
         <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="X9" s="1"/>
+        <v>26</v>
+      </c>
+      <c r="AH9" s="1"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
         <v>25</v>
@@ -1548,26 +1782,44 @@
         <v>8</v>
       </c>
       <c r="I10" s="3">
-        <v>0</v>
-      </c>
-      <c r="J10" s="3"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="J10" s="3">
+        <v>0</v>
+      </c>
+      <c r="K10" s="3">
+        <v>18</v>
+      </c>
+      <c r="L10" s="3">
+        <v>18</v>
+      </c>
       <c r="M10" s="3"/>
-      <c r="N10" s="8"/>
+      <c r="N10" s="3">
+        <v>14</v>
+      </c>
       <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="8"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="3"/>
       <c r="R10" s="3"/>
-      <c r="S10" s="3"/>
-      <c r="V10" s="1"/>
-      <c r="W10" s="1">
+      <c r="S10" s="8"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="3"/>
+      <c r="W10" s="3"/>
+      <c r="X10" s="3"/>
+      <c r="Y10" s="3"/>
+      <c r="Z10" s="3"/>
+      <c r="AA10" s="8"/>
+      <c r="AB10" s="3"/>
+      <c r="AC10" s="3"/>
+      <c r="AF10" s="1"/>
+      <c r="AG10" s="1">
         <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="X10" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="AH10" s="1"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
@@ -1593,46 +1845,74 @@
         <v>935</v>
       </c>
       <c r="I11" s="1">
-        <v>0</v>
+        <v>807</v>
       </c>
       <c r="J11" s="1">
+        <v>0</v>
+      </c>
+      <c r="K11" s="1">
+        <v>801</v>
+      </c>
+      <c r="L11" s="1">
+        <v>806</v>
+      </c>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1">
+        <v>779</v>
+      </c>
+      <c r="O11" s="1">
         <v>967</v>
       </c>
-      <c r="K11" s="11">
+      <c r="P11" s="11">
         <v>947</v>
       </c>
-      <c r="L11" s="5">
+      <c r="Q11" s="5">
         <v>937</v>
       </c>
-      <c r="M11" s="5">
+      <c r="R11" s="5">
         <v>869</v>
       </c>
-      <c r="N11" s="7">
+      <c r="S11" s="7">
         <v>830</v>
       </c>
-      <c r="O11" s="1">
+      <c r="T11" s="5">
+        <v>988</v>
+      </c>
+      <c r="U11" s="5">
+        <v>958</v>
+      </c>
+      <c r="V11" s="1">
         <v>985</v>
       </c>
-      <c r="P11" s="1">
+      <c r="W11" s="1">
+        <v>837</v>
+      </c>
+      <c r="X11" s="1">
+        <v>981</v>
+      </c>
+      <c r="Y11" s="1">
         <v>1007</v>
       </c>
-      <c r="Q11" s="7">
+      <c r="Z11" s="1">
+        <v>918</v>
+      </c>
+      <c r="AA11" s="7">
         <v>964</v>
       </c>
-      <c r="R11" s="1">
+      <c r="AB11" s="1">
         <v>966</v>
       </c>
-      <c r="S11" s="1">
+      <c r="AC11" s="1">
         <v>966</v>
       </c>
-      <c r="V11" s="1"/>
-      <c r="W11" s="1">
+      <c r="AF11" s="1"/>
+      <c r="AG11" s="1">
         <f t="shared" si="0"/>
         <v>1007</v>
       </c>
-      <c r="X11" s="1"/>
+      <c r="AH11" s="1"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="5" t="s">
         <v>24</v>
@@ -1656,26 +1936,44 @@
         <v>941</v>
       </c>
       <c r="I12" s="1">
-        <v>0</v>
-      </c>
-      <c r="J12" s="1"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="7"/>
+        <v>807</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1">
+        <v>806</v>
+      </c>
+      <c r="L12" s="1">
+        <v>813</v>
+      </c>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1">
+        <v>569</v>
+      </c>
       <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="1"/>
-      <c r="S12" s="1"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5"/>
+      <c r="S12" s="7"/>
+      <c r="T12" s="5"/>
+      <c r="U12" s="5"/>
       <c r="V12" s="1"/>
-      <c r="W12" s="1">
+      <c r="W12" s="1"/>
+      <c r="X12" s="1"/>
+      <c r="Y12" s="1"/>
+      <c r="Z12" s="1"/>
+      <c r="AA12" s="7"/>
+      <c r="AB12" s="1"/>
+      <c r="AC12" s="1"/>
+      <c r="AF12" s="1"/>
+      <c r="AG12" s="1">
         <f t="shared" si="0"/>
         <v>964</v>
       </c>
-      <c r="X12" s="1"/>
+      <c r="AH12" s="1"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3" t="s">
         <v>25</v>
@@ -1699,26 +1997,44 @@
         <v>613</v>
       </c>
       <c r="I13" s="3">
-        <v>0</v>
-      </c>
-      <c r="J13" s="3"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="3"/>
+        <v>453</v>
+      </c>
+      <c r="J13" s="3">
+        <v>0</v>
+      </c>
+      <c r="K13" s="3">
+        <v>787</v>
+      </c>
+      <c r="L13" s="3">
+        <v>795</v>
+      </c>
       <c r="M13" s="3"/>
-      <c r="N13" s="8"/>
+      <c r="N13" s="3">
+        <v>159</v>
+      </c>
       <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="8"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="3"/>
       <c r="R13" s="3"/>
-      <c r="S13" s="3"/>
-      <c r="V13" s="1"/>
-      <c r="W13" s="1">
+      <c r="S13" s="8"/>
+      <c r="T13" s="3"/>
+      <c r="U13" s="3"/>
+      <c r="V13" s="3"/>
+      <c r="W13" s="3"/>
+      <c r="X13" s="3"/>
+      <c r="Y13" s="3"/>
+      <c r="Z13" s="3"/>
+      <c r="AA13" s="8"/>
+      <c r="AB13" s="3"/>
+      <c r="AC13" s="3"/>
+      <c r="AF13" s="1"/>
+      <c r="AG13" s="1">
         <f t="shared" si="0"/>
         <v>914</v>
       </c>
-      <c r="X13" s="1"/>
+      <c r="AH13" s="1"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -1744,46 +2060,72 @@
         <v>411</v>
       </c>
       <c r="I14" s="1">
-        <v>0</v>
+        <v>541</v>
       </c>
       <c r="J14" s="1">
+        <v>0</v>
+      </c>
+      <c r="K14" s="1">
+        <v>553</v>
+      </c>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1">
+        <v>0</v>
+      </c>
+      <c r="O14" s="1">
         <v>497</v>
       </c>
-      <c r="K14" s="11">
+      <c r="P14" s="11">
         <v>927</v>
       </c>
-      <c r="L14" s="5">
+      <c r="Q14" s="5">
         <v>445</v>
       </c>
-      <c r="M14" s="5">
+      <c r="R14" s="5">
         <v>633</v>
       </c>
-      <c r="N14" s="7">
+      <c r="S14" s="7">
         <v>263</v>
       </c>
-      <c r="O14" s="1">
+      <c r="T14" s="5">
+        <v>938</v>
+      </c>
+      <c r="U14" s="5">
+        <v>967</v>
+      </c>
+      <c r="V14" s="1">
         <v>998</v>
       </c>
-      <c r="P14" s="1">
+      <c r="W14" s="1">
+        <v>937</v>
+      </c>
+      <c r="X14" s="1">
+        <v>866</v>
+      </c>
+      <c r="Y14" s="1">
         <v>633</v>
       </c>
-      <c r="Q14" s="7">
+      <c r="Z14" s="1">
+        <v>929</v>
+      </c>
+      <c r="AA14" s="7">
         <v>799</v>
       </c>
-      <c r="R14" s="1">
+      <c r="AB14" s="1">
         <v>962</v>
       </c>
-      <c r="S14" s="1">
+      <c r="AC14" s="1">
         <v>972</v>
       </c>
-      <c r="V14" s="1"/>
-      <c r="W14" s="1">
+      <c r="AF14" s="1"/>
+      <c r="AG14" s="1">
         <f t="shared" si="0"/>
         <v>998</v>
       </c>
-      <c r="X14" s="1"/>
+      <c r="AH14" s="1"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="5" t="s">
         <v>24</v>
@@ -1807,25 +2149,41 @@
         <v>401</v>
       </c>
       <c r="I15" s="1">
-        <v>0</v>
-      </c>
-      <c r="J15" s="1"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="7"/>
+        <v>611</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0</v>
+      </c>
+      <c r="K15" s="1">
+        <v>768</v>
+      </c>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1">
+        <v>0</v>
+      </c>
       <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="1"/>
-      <c r="S15" s="1"/>
-      <c r="T15" s="1"/>
-      <c r="U15" s="1"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="5"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="5"/>
+      <c r="U15" s="5"/>
       <c r="V15" s="1"/>
       <c r="W15" s="1"/>
       <c r="X15" s="1"/>
+      <c r="Y15" s="1"/>
+      <c r="Z15" s="1"/>
+      <c r="AA15" s="7"/>
+      <c r="AB15" s="1"/>
+      <c r="AC15" s="1"/>
+      <c r="AD15" s="1"/>
+      <c r="AE15" s="1"/>
+      <c r="AF15" s="1"/>
+      <c r="AG15" s="1"/>
+      <c r="AH15" s="1"/>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="5" t="s">
         <v>25</v>
@@ -1849,25 +2207,41 @@
         <v>946</v>
       </c>
       <c r="I16" s="1">
-        <v>0</v>
-      </c>
-      <c r="J16" s="1"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="7"/>
+        <v>805</v>
+      </c>
+      <c r="J16" s="1">
+        <v>0</v>
+      </c>
+      <c r="K16" s="1">
+        <v>806</v>
+      </c>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1">
+        <v>0</v>
+      </c>
       <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="7"/>
-      <c r="R16" s="1"/>
-      <c r="S16" s="1"/>
-      <c r="T16" s="1"/>
-      <c r="U16" s="1"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="5"/>
+      <c r="S16" s="7"/>
+      <c r="T16" s="5"/>
+      <c r="U16" s="5"/>
       <c r="V16" s="1"/>
       <c r="W16" s="1"/>
       <c r="X16" s="1"/>
+      <c r="Y16" s="1"/>
+      <c r="Z16" s="1"/>
+      <c r="AA16" s="7"/>
+      <c r="AB16" s="1"/>
+      <c r="AC16" s="1"/>
+      <c r="AD16" s="1"/>
+      <c r="AE16" s="1"/>
+      <c r="AF16" s="1"/>
+      <c r="AG16" s="1"/>
+      <c r="AH16" s="1"/>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1892,8 +2266,18 @@
       <c r="V17" s="1"/>
       <c r="W17" s="1"/>
       <c r="X17" s="1"/>
+      <c r="Y17" s="1"/>
+      <c r="Z17" s="1"/>
+      <c r="AA17" s="1"/>
+      <c r="AB17" s="1"/>
+      <c r="AC17" s="1"/>
+      <c r="AD17" s="1"/>
+      <c r="AE17" s="1"/>
+      <c r="AF17" s="1"/>
+      <c r="AG17" s="1"/>
+      <c r="AH17" s="1"/>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1918,8 +2302,18 @@
       <c r="V18" s="1"/>
       <c r="W18" s="1"/>
       <c r="X18" s="1"/>
+      <c r="Y18" s="1"/>
+      <c r="Z18" s="1"/>
+      <c r="AA18" s="1"/>
+      <c r="AB18" s="1"/>
+      <c r="AC18" s="1"/>
+      <c r="AD18" s="1"/>
+      <c r="AE18" s="1"/>
+      <c r="AF18" s="1"/>
+      <c r="AG18" s="1"/>
+      <c r="AH18" s="1"/>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1944,10 +2338,20 @@
       <c r="V19" s="1"/>
       <c r="W19" s="1"/>
       <c r="X19" s="1"/>
+      <c r="Y19" s="1"/>
+      <c r="Z19" s="1"/>
+      <c r="AA19" s="1"/>
+      <c r="AB19" s="1"/>
+      <c r="AC19" s="1"/>
+      <c r="AD19" s="1"/>
+      <c r="AE19" s="1"/>
+      <c r="AF19" s="1"/>
+      <c r="AG19" s="1"/>
+      <c r="AH19" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:I2">
-    <cfRule type="colorScale" priority="16">
+  <conditionalFormatting sqref="C2:L2">
+    <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1958,8 +2362,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:I3">
-    <cfRule type="colorScale" priority="13">
+  <conditionalFormatting sqref="C3:L3">
+    <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1970,8 +2374,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C4:I4">
-    <cfRule type="colorScale" priority="14">
+  <conditionalFormatting sqref="C4:L4">
+    <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1982,8 +2386,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C5:I5">
-    <cfRule type="colorScale" priority="12">
+  <conditionalFormatting sqref="C5:L5">
+    <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1994,8 +2398,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C6:I6">
-    <cfRule type="colorScale" priority="11">
+  <conditionalFormatting sqref="C6:L6">
+    <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2006,8 +2410,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7:I7">
-    <cfRule type="colorScale" priority="10">
+  <conditionalFormatting sqref="C7:L7">
+    <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2018,8 +2422,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8:I8">
-    <cfRule type="colorScale" priority="9">
+  <conditionalFormatting sqref="C8:L8">
+    <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2030,8 +2434,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C9:I9">
-    <cfRule type="colorScale" priority="8">
+  <conditionalFormatting sqref="C9:L9">
+    <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2042,8 +2446,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C10:I10">
-    <cfRule type="colorScale" priority="7">
+  <conditionalFormatting sqref="C10:L10">
+    <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2054,8 +2458,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C11:I11">
-    <cfRule type="colorScale" priority="6">
+  <conditionalFormatting sqref="C11:L11">
+    <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2066,8 +2470,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C12:I12">
-    <cfRule type="colorScale" priority="5">
+  <conditionalFormatting sqref="C12:L12">
+    <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2078,8 +2482,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C13:I13">
-    <cfRule type="colorScale" priority="4">
+  <conditionalFormatting sqref="C13:L13">
+    <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2090,8 +2494,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C14:I14">
-    <cfRule type="colorScale" priority="3">
+  <conditionalFormatting sqref="C14:L14">
+    <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2102,8 +2506,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C15:I15">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="C15:M15">
+    <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2114,8 +2518,32 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C16:I16">
+  <conditionalFormatting sqref="C16:M16">
+    <cfRule type="colorScale" priority="34">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N15">
     <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N16">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>

<commit_message>
Adding some references, some editing and finish future work and start implementation chapter
</commit_message>
<xml_diff>
--- a/tncData.xlsx
+++ b/tncData.xlsx
@@ -15,6 +15,7 @@
     <sheet name="tncData" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -60,9 +61,6 @@
     <t>PK-232</t>
   </si>
   <si>
-    <t>Goertzel</t>
-  </si>
-  <si>
     <t>AGWPE</t>
   </si>
   <si>
@@ -135,7 +133,10 @@
     <t>Goertzel Optimized window</t>
   </si>
   <si>
-    <t>Threaded Goertzel</t>
+    <t>Derivative</t>
+  </si>
+  <si>
+    <t>Goertzel (100%)</t>
   </si>
 </sst>
 </file>
@@ -1057,8 +1058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="U18" sqref="U18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1073,10 +1074,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -1088,31 +1089,31 @@
         <v>3</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="M1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="P1" s="9" t="s">
         <v>7</v>
@@ -1127,19 +1128,19 @@
         <v>11</v>
       </c>
       <c r="T1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="U1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="V1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="X1" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="Y1" s="3" t="s">
         <v>10</v>
@@ -1148,34 +1149,34 @@
         <v>12</v>
       </c>
       <c r="AA1" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AB1" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="AC1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="AF1" s="1"/>
       <c r="AG1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH1" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" s="10">
         <v>40</v>
       </c>
       <c r="D2" s="4">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E2" s="4">
         <v>40</v>
@@ -1186,22 +1187,22 @@
       <c r="G2" s="4">
         <v>0</v>
       </c>
-      <c r="H2" s="4">
-        <v>40</v>
-      </c>
+      <c r="H2" s="4"/>
       <c r="I2" s="4">
         <v>40</v>
       </c>
       <c r="J2" s="4">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="K2" s="4">
         <v>40</v>
       </c>
       <c r="L2" s="4">
-        <v>40</v>
-      </c>
-      <c r="M2" s="4"/>
+        <v>0</v>
+      </c>
+      <c r="M2" s="4">
+        <v>40</v>
+      </c>
       <c r="N2" s="4">
         <v>40</v>
       </c>
@@ -1262,13 +1263,13 @@
     <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" s="11">
         <v>40</v>
       </c>
       <c r="D3" s="5">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="E3" s="5">
         <v>0</v>
@@ -1277,16 +1278,14 @@
         <v>0</v>
       </c>
       <c r="G3" s="5">
-        <v>40</v>
-      </c>
-      <c r="H3" s="5">
-        <v>40</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H3" s="5"/>
       <c r="I3" s="5">
         <v>40</v>
       </c>
       <c r="J3" s="5">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="K3" s="5">
         <v>40</v>
@@ -1294,7 +1293,9 @@
       <c r="L3" s="5">
         <v>40</v>
       </c>
-      <c r="M3" s="5"/>
+      <c r="M3" s="5">
+        <v>40</v>
+      </c>
       <c r="N3" s="5">
         <v>40</v>
       </c>
@@ -1325,13 +1326,13 @@
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="9">
         <v>40</v>
       </c>
       <c r="D4" s="3">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E4" s="3">
         <v>40</v>
@@ -1340,26 +1341,26 @@
         <v>0</v>
       </c>
       <c r="G4" s="3">
+        <v>0</v>
+      </c>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3">
+        <v>40</v>
+      </c>
+      <c r="J4" s="3">
+        <v>40</v>
+      </c>
+      <c r="K4" s="3">
+        <v>0</v>
+      </c>
+      <c r="L4" s="3">
         <v>39</v>
       </c>
-      <c r="H4" s="3">
-        <v>40</v>
-      </c>
-      <c r="I4" s="3">
-        <v>40</v>
-      </c>
-      <c r="J4" s="3">
-        <v>0</v>
-      </c>
-      <c r="K4" s="3">
-        <v>40</v>
-      </c>
-      <c r="L4" s="3">
-        <v>40</v>
-      </c>
-      <c r="M4" s="3"/>
+      <c r="M4" s="3">
+        <v>40</v>
+      </c>
       <c r="N4" s="3">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="O4" s="3"/>
       <c r="P4" s="9"/>
@@ -1387,10 +1388,10 @@
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" s="11">
         <v>200</v>
@@ -1407,22 +1408,22 @@
       <c r="G5" s="1">
         <v>0</v>
       </c>
-      <c r="H5" s="1">
-        <v>200</v>
-      </c>
+      <c r="H5" s="1"/>
       <c r="I5" s="1">
         <v>200</v>
       </c>
       <c r="J5" s="1">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="K5" s="1">
         <v>200</v>
       </c>
       <c r="L5" s="1">
-        <v>200</v>
-      </c>
-      <c r="M5" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="M5" s="1">
+        <v>200</v>
+      </c>
       <c r="N5" s="1">
         <v>200</v>
       </c>
@@ -1481,13 +1482,13 @@
     <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" s="11">
         <v>200</v>
       </c>
       <c r="D6" s="1">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="E6" s="1">
         <v>200</v>
@@ -1496,16 +1497,14 @@
         <v>0</v>
       </c>
       <c r="G6" s="1">
-        <v>200</v>
-      </c>
-      <c r="H6" s="1">
-        <v>200</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H6" s="1"/>
       <c r="I6" s="1">
         <v>200</v>
       </c>
       <c r="J6" s="1">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="K6" s="1">
         <v>200</v>
@@ -1513,7 +1512,9 @@
       <c r="L6" s="1">
         <v>200</v>
       </c>
-      <c r="M6" s="1"/>
+      <c r="M6" s="1">
+        <v>200</v>
+      </c>
       <c r="N6" s="1">
         <v>200</v>
       </c>
@@ -1544,13 +1545,13 @@
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" s="9">
         <v>200</v>
       </c>
       <c r="D7" s="3">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="E7" s="3">
         <v>200</v>
@@ -1559,16 +1560,14 @@
         <v>0</v>
       </c>
       <c r="G7" s="3">
-        <v>200</v>
-      </c>
-      <c r="H7" s="3">
-        <v>200</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H7" s="3"/>
       <c r="I7" s="3">
         <v>200</v>
       </c>
       <c r="J7" s="3">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="K7" s="3">
         <v>200</v>
@@ -1576,7 +1575,9 @@
       <c r="L7" s="3">
         <v>200</v>
       </c>
-      <c r="M7" s="3"/>
+      <c r="M7" s="3">
+        <v>200</v>
+      </c>
       <c r="N7" s="3">
         <v>200</v>
       </c>
@@ -1606,10 +1607,10 @@
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" s="11">
         <v>24</v>
@@ -1626,24 +1627,24 @@
       <c r="G8" s="1">
         <v>0</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="1"/>
+      <c r="I8" s="1">
         <v>17</v>
       </c>
-      <c r="I8" s="1">
+      <c r="J8" s="1">
         <v>25</v>
       </c>
-      <c r="J8" s="1">
-        <v>0</v>
-      </c>
       <c r="K8" s="1">
+        <v>21</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0</v>
+      </c>
+      <c r="M8" s="1">
         <v>27</v>
       </c>
-      <c r="L8" s="1">
+      <c r="N8" s="1">
         <v>27</v>
-      </c>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1">
-        <v>21</v>
       </c>
       <c r="O8" s="1">
         <v>21</v>
@@ -1700,7 +1701,7 @@
     <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="11">
         <v>24</v>
@@ -1715,26 +1716,26 @@
         <v>0</v>
       </c>
       <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1">
+        <v>21</v>
+      </c>
+      <c r="J9" s="1">
+        <v>23</v>
+      </c>
+      <c r="K9" s="1">
+        <v>23</v>
+      </c>
+      <c r="L9" s="1">
         <v>17</v>
       </c>
-      <c r="H9" s="1">
-        <v>21</v>
-      </c>
-      <c r="I9" s="1">
-        <v>23</v>
-      </c>
-      <c r="J9" s="1">
-        <v>0</v>
-      </c>
-      <c r="K9" s="1">
+      <c r="M9" s="1">
         <v>26</v>
       </c>
-      <c r="L9" s="1">
+      <c r="N9" s="1">
         <v>26</v>
-      </c>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1">
-        <v>23</v>
       </c>
       <c r="O9" s="1"/>
       <c r="P9" s="11"/>
@@ -1761,7 +1762,7 @@
     <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="9">
         <v>11</v>
@@ -1776,26 +1777,26 @@
         <v>0</v>
       </c>
       <c r="G10" s="3">
-        <v>6</v>
-      </c>
-      <c r="H10" s="3">
-        <v>8</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H10" s="3"/>
       <c r="I10" s="3">
         <v>8</v>
       </c>
       <c r="J10" s="3">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K10" s="3">
+        <v>14</v>
+      </c>
+      <c r="L10" s="3">
+        <v>6</v>
+      </c>
+      <c r="M10" s="3">
         <v>18</v>
       </c>
-      <c r="L10" s="3">
+      <c r="N10" s="3">
         <v>18</v>
-      </c>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3">
-        <v>14</v>
       </c>
       <c r="O10" s="3"/>
       <c r="P10" s="9"/>
@@ -1821,16 +1822,16 @@
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" s="11">
         <v>946</v>
       </c>
       <c r="D11" s="1">
-        <v>64</v>
+        <v>460</v>
       </c>
       <c r="E11" s="1">
         <v>568</v>
@@ -1841,24 +1842,24 @@
       <c r="G11" s="1">
         <v>0</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11" s="1"/>
+      <c r="I11" s="1">
         <v>935</v>
       </c>
-      <c r="I11" s="1">
-        <v>807</v>
-      </c>
       <c r="J11" s="1">
-        <v>0</v>
+        <v>965</v>
       </c>
       <c r="K11" s="1">
+        <v>779</v>
+      </c>
+      <c r="L11" s="1">
+        <v>0</v>
+      </c>
+      <c r="M11" s="1">
         <v>801</v>
       </c>
-      <c r="L11" s="1">
+      <c r="N11" s="1">
         <v>806</v>
-      </c>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1">
-        <v>779</v>
       </c>
       <c r="O11" s="1">
         <v>967</v>
@@ -1915,41 +1916,41 @@
     <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12" s="11">
         <v>964</v>
       </c>
       <c r="D12" s="1">
-        <v>74</v>
+        <v>460</v>
       </c>
       <c r="E12" s="1">
         <v>151</v>
       </c>
       <c r="F12" s="1">
-        <v>0</v>
+        <v>298</v>
       </c>
       <c r="G12" s="1">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1">
+        <v>941</v>
+      </c>
+      <c r="J12" s="1">
+        <v>807</v>
+      </c>
+      <c r="K12" s="1">
+        <v>569</v>
+      </c>
+      <c r="L12" s="1">
         <v>938</v>
       </c>
-      <c r="H12" s="1">
-        <v>941</v>
-      </c>
-      <c r="I12" s="1">
-        <v>807</v>
-      </c>
-      <c r="J12" s="1">
-        <v>0</v>
-      </c>
-      <c r="K12" s="1">
+      <c r="M12" s="1">
         <v>806</v>
       </c>
-      <c r="L12" s="1">
+      <c r="N12" s="1">
         <v>813</v>
-      </c>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1">
-        <v>569</v>
       </c>
       <c r="O12" s="1"/>
       <c r="P12" s="11"/>
@@ -1976,7 +1977,7 @@
     <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" s="9">
         <v>914</v>
@@ -1991,26 +1992,26 @@
         <v>0</v>
       </c>
       <c r="G13" s="3">
+        <v>0</v>
+      </c>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3">
+        <v>613</v>
+      </c>
+      <c r="J13" s="3">
+        <v>453</v>
+      </c>
+      <c r="K13" s="3">
+        <v>159</v>
+      </c>
+      <c r="L13" s="3">
         <v>481</v>
       </c>
-      <c r="H13" s="3">
-        <v>613</v>
-      </c>
-      <c r="I13" s="3">
-        <v>453</v>
-      </c>
-      <c r="J13" s="3">
-        <v>0</v>
-      </c>
-      <c r="K13" s="3">
+      <c r="M13" s="3">
         <v>787</v>
       </c>
-      <c r="L13" s="3">
+      <c r="N13" s="3">
         <v>795</v>
-      </c>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3">
-        <v>159</v>
       </c>
       <c r="O13" s="3"/>
       <c r="P13" s="9"/>
@@ -2036,10 +2037,10 @@
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" s="11">
         <v>639</v>
@@ -2056,23 +2057,23 @@
       <c r="G14" s="1">
         <v>0</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H14" s="1"/>
+      <c r="I14" s="1">
         <v>411</v>
       </c>
-      <c r="I14" s="1">
+      <c r="J14" s="1">
         <v>541</v>
       </c>
-      <c r="J14" s="1">
-        <v>0</v>
-      </c>
       <c r="K14" s="1">
+        <v>0</v>
+      </c>
+      <c r="L14" s="1">
+        <v>0</v>
+      </c>
+      <c r="M14" s="1">
         <v>553</v>
       </c>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1">
-        <v>0</v>
-      </c>
+      <c r="N14" s="1"/>
       <c r="O14" s="1">
         <v>497</v>
       </c>
@@ -2128,7 +2129,7 @@
     <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" s="11">
         <v>872</v>
@@ -2143,25 +2144,25 @@
         <v>0</v>
       </c>
       <c r="G15" s="1">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1">
+        <v>401</v>
+      </c>
+      <c r="J15" s="1">
+        <v>611</v>
+      </c>
+      <c r="K15" s="1">
+        <v>0</v>
+      </c>
+      <c r="L15" s="1">
         <v>939</v>
       </c>
-      <c r="H15" s="1">
-        <v>401</v>
-      </c>
-      <c r="I15" s="1">
-        <v>611</v>
-      </c>
-      <c r="J15" s="1">
-        <v>0</v>
-      </c>
-      <c r="K15" s="1">
+      <c r="M15" s="1">
         <v>768</v>
       </c>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1">
-        <v>0</v>
-      </c>
+      <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="11"/>
       <c r="Q15" s="5"/>
@@ -2186,7 +2187,7 @@
     <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C16" s="11">
         <v>958</v>
@@ -2201,25 +2202,25 @@
         <v>0</v>
       </c>
       <c r="G16" s="1">
+        <v>0</v>
+      </c>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1">
         <v>946</v>
       </c>
-      <c r="H16" s="1">
+      <c r="J16" s="1">
+        <v>805</v>
+      </c>
+      <c r="K16" s="1">
+        <v>0</v>
+      </c>
+      <c r="L16" s="1">
         <v>946</v>
       </c>
-      <c r="I16" s="1">
-        <v>805</v>
-      </c>
-      <c r="J16" s="1">
-        <v>0</v>
-      </c>
-      <c r="K16" s="1">
+      <c r="M16" s="1">
         <v>806</v>
       </c>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1">
-        <v>0</v>
-      </c>
+      <c r="N16" s="1"/>
       <c r="O16" s="1"/>
       <c r="P16" s="11"/>
       <c r="Q16" s="5"/>
@@ -2350,7 +2351,19 @@
       <c r="AH19" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:L2">
+  <conditionalFormatting sqref="G2">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -2362,7 +2375,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:L3">
+  <conditionalFormatting sqref="G4">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
@@ -2374,7 +2387,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C4:L4">
+  <conditionalFormatting sqref="G5">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
@@ -2386,7 +2399,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C5:L5">
+  <conditionalFormatting sqref="G6">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
@@ -2398,7 +2411,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C6:L6">
+  <conditionalFormatting sqref="G7">
     <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
@@ -2410,7 +2423,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7:L7">
+  <conditionalFormatting sqref="G8">
     <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
@@ -2422,7 +2435,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8:L8">
+  <conditionalFormatting sqref="G9">
     <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
@@ -2434,7 +2447,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C9:L9">
+  <conditionalFormatting sqref="G10">
     <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
@@ -2446,7 +2459,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C10:L10">
+  <conditionalFormatting sqref="G11">
     <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
@@ -2458,7 +2471,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C11:L11">
+  <conditionalFormatting sqref="G12">
     <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="min"/>
@@ -2470,7 +2483,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C12:L12">
+  <conditionalFormatting sqref="G13">
     <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min"/>
@@ -2482,7 +2495,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C13:L13">
+  <conditionalFormatting sqref="G14">
     <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min"/>
@@ -2494,7 +2507,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C14:L14">
+  <conditionalFormatting sqref="G15">
     <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
@@ -2506,7 +2519,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C15:M15">
+  <conditionalFormatting sqref="G16">
     <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="min"/>
@@ -2518,19 +2531,187 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C16:M16">
-    <cfRule type="colorScale" priority="34">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N15">
+  <conditionalFormatting sqref="I2:J2">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3:J3">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4:J4">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I5:J5">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I6:J6">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I7:J7">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I8:J8">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I9:J9">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I10:J10">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I11:J11">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I12:J12">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I13:J13">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I14:J14">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I15:J15">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I16:J16">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K15">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -2542,8 +2723,188 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N16">
+  <conditionalFormatting sqref="K16">
     <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:F2 H2 L2:N2">
+    <cfRule type="colorScale" priority="67">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:F3 H3 L3:N3">
+    <cfRule type="colorScale" priority="71">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C4:F4 H4 L4:N4">
+    <cfRule type="colorScale" priority="75">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5:F5 H5 L5:N5">
+    <cfRule type="colorScale" priority="79">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C6:F6 H6 L6:N6">
+    <cfRule type="colorScale" priority="83">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7:F7 H7 L7:N7">
+    <cfRule type="colorScale" priority="87">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8:F8 H8 L8:N8">
+    <cfRule type="colorScale" priority="91">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9:F9 H9 L9:N9">
+    <cfRule type="colorScale" priority="95">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10:F10 H10 L10:N10">
+    <cfRule type="colorScale" priority="99">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11:F11 H11 L11:N11">
+    <cfRule type="colorScale" priority="103">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12:F12 H12 L12:N12">
+    <cfRule type="colorScale" priority="107">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13:F13 H13 L13:N13">
+    <cfRule type="colorScale" priority="111">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14:F14 H14 L14:N14">
+    <cfRule type="colorScale" priority="115">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15:F15 H15 L15:N15">
+    <cfRule type="colorScale" priority="124">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C16:F16 H16 L16:N16">
+    <cfRule type="colorScale" priority="127">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>

<commit_message>
Implementation section and beginnings of result section to see how images look in document
</commit_message>
<xml_diff>
--- a/tncData.xlsx
+++ b/tncData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="12180"/>
   </bookViews>
   <sheets>
     <sheet name="tncData" sheetId="1" r:id="rId1"/>
@@ -705,9 +705,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -733,6 +730,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1058,8 +1058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1070,91 +1070,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="P1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="S1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="T1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="U1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="V1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="W1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="X1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Y1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="Z1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="AA1" s="8" t="s">
+      <c r="AA1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AB1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AC1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="AF1" s="1"/>
@@ -1166,89 +1166,91 @@
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="10">
-        <v>40</v>
-      </c>
-      <c r="D2" s="4">
+      <c r="C2" s="9">
+        <v>40</v>
+      </c>
+      <c r="D2" s="3">
         <v>35</v>
       </c>
-      <c r="E2" s="4">
-        <v>40</v>
-      </c>
-      <c r="F2" s="4">
+      <c r="E2" s="3">
+        <v>40</v>
+      </c>
+      <c r="F2" s="3">
         <v>39</v>
       </c>
-      <c r="G2" s="4">
-        <v>0</v>
-      </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4">
-        <v>40</v>
-      </c>
-      <c r="J2" s="4">
-        <v>40</v>
-      </c>
-      <c r="K2" s="4">
-        <v>40</v>
-      </c>
-      <c r="L2" s="4">
-        <v>0</v>
-      </c>
-      <c r="M2" s="4">
-        <v>40</v>
-      </c>
-      <c r="N2" s="4">
-        <v>40</v>
-      </c>
-      <c r="O2" s="4">
-        <v>40</v>
-      </c>
-      <c r="P2" s="10">
-        <v>40</v>
-      </c>
-      <c r="Q2" s="4">
-        <v>40</v>
-      </c>
-      <c r="R2" s="4">
+      <c r="G2" s="3">
+        <v>3</v>
+      </c>
+      <c r="H2" s="3">
+        <v>40</v>
+      </c>
+      <c r="I2" s="3">
+        <v>40</v>
+      </c>
+      <c r="J2" s="3">
+        <v>40</v>
+      </c>
+      <c r="K2" s="3">
+        <v>40</v>
+      </c>
+      <c r="L2" s="3">
+        <v>0</v>
+      </c>
+      <c r="M2" s="3">
+        <v>40</v>
+      </c>
+      <c r="N2" s="3">
+        <v>40</v>
+      </c>
+      <c r="O2" s="3">
+        <v>40</v>
+      </c>
+      <c r="P2" s="9">
+        <v>40</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>40</v>
+      </c>
+      <c r="R2" s="3">
         <v>39</v>
       </c>
-      <c r="S2" s="6">
-        <v>40</v>
-      </c>
-      <c r="T2" s="4">
-        <v>40</v>
-      </c>
-      <c r="U2" s="4">
-        <v>40</v>
-      </c>
-      <c r="V2" s="4">
-        <v>40</v>
-      </c>
-      <c r="W2" s="4">
-        <v>40</v>
-      </c>
-      <c r="X2" s="4">
-        <v>40</v>
-      </c>
-      <c r="Y2" s="4">
-        <v>40</v>
-      </c>
-      <c r="Z2" s="4">
-        <v>40</v>
-      </c>
-      <c r="AA2" s="6">
-        <v>40</v>
-      </c>
-      <c r="AB2" s="4">
-        <v>40</v>
-      </c>
-      <c r="AC2" s="4">
+      <c r="S2" s="5">
+        <v>40</v>
+      </c>
+      <c r="T2" s="3">
+        <v>40</v>
+      </c>
+      <c r="U2" s="3">
+        <v>40</v>
+      </c>
+      <c r="V2" s="3">
+        <v>40</v>
+      </c>
+      <c r="W2" s="3">
+        <v>40</v>
+      </c>
+      <c r="X2" s="3">
+        <v>40</v>
+      </c>
+      <c r="Y2" s="3">
+        <v>40</v>
+      </c>
+      <c r="Z2" s="3">
+        <v>40</v>
+      </c>
+      <c r="AA2" s="5">
+        <v>40</v>
+      </c>
+      <c r="AB2" s="3">
+        <v>40</v>
+      </c>
+      <c r="AC2" s="3">
         <v>40</v>
       </c>
       <c r="AF2" s="1"/>
@@ -1261,59 +1263,61 @@
       </c>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5" t="s">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="11">
-        <v>40</v>
-      </c>
-      <c r="D3" s="5">
-        <v>35</v>
-      </c>
-      <c r="E3" s="5">
-        <v>0</v>
-      </c>
-      <c r="F3" s="5">
-        <v>0</v>
-      </c>
-      <c r="G3" s="5">
-        <v>0</v>
-      </c>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5">
-        <v>40</v>
-      </c>
-      <c r="J3" s="5">
-        <v>40</v>
-      </c>
-      <c r="K3" s="5">
-        <v>40</v>
-      </c>
-      <c r="L3" s="5">
-        <v>40</v>
-      </c>
-      <c r="M3" s="5">
-        <v>40</v>
-      </c>
-      <c r="N3" s="5">
-        <v>40</v>
-      </c>
-      <c r="O3" s="5"/>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="7"/>
-      <c r="T3" s="5"/>
-      <c r="U3" s="5"/>
-      <c r="V3" s="5"/>
-      <c r="W3" s="5"/>
-      <c r="X3" s="5"/>
-      <c r="Y3" s="5"/>
-      <c r="Z3" s="5"/>
-      <c r="AA3" s="7"/>
-      <c r="AB3" s="5"/>
-      <c r="AC3" s="5"/>
+      <c r="C3" s="10">
+        <v>40</v>
+      </c>
+      <c r="D3" s="4">
+        <v>19</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0</v>
+      </c>
+      <c r="H3" s="4">
+        <v>33</v>
+      </c>
+      <c r="I3" s="4">
+        <v>40</v>
+      </c>
+      <c r="J3" s="4">
+        <v>40</v>
+      </c>
+      <c r="K3" s="4">
+        <v>40</v>
+      </c>
+      <c r="L3" s="4">
+        <v>40</v>
+      </c>
+      <c r="M3" s="4">
+        <v>28</v>
+      </c>
+      <c r="N3" s="4">
+        <v>40</v>
+      </c>
+      <c r="O3" s="4"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
+      <c r="V3" s="4"/>
+      <c r="W3" s="4"/>
+      <c r="X3" s="4"/>
+      <c r="Y3" s="4"/>
+      <c r="Z3" s="4"/>
+      <c r="AA3" s="6"/>
+      <c r="AB3" s="4"/>
+      <c r="AC3" s="4"/>
       <c r="AF3" s="1"/>
       <c r="AG3" s="1">
         <f t="shared" ref="AG3:AG14" si="0">MAX(C3:AF3)</f>
@@ -1324,59 +1328,61 @@
       </c>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="9">
-        <v>40</v>
-      </c>
-      <c r="D4" s="3">
+      <c r="C4" s="8">
+        <v>40</v>
+      </c>
+      <c r="D4" s="2">
         <v>12</v>
       </c>
-      <c r="E4" s="3">
-        <v>40</v>
-      </c>
-      <c r="F4" s="3">
-        <v>0</v>
-      </c>
-      <c r="G4" s="3">
-        <v>0</v>
-      </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3">
-        <v>40</v>
-      </c>
-      <c r="J4" s="3">
-        <v>40</v>
-      </c>
-      <c r="K4" s="3">
-        <v>0</v>
-      </c>
-      <c r="L4" s="3">
+      <c r="E4" s="2">
+        <v>40</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2">
+        <v>14</v>
+      </c>
+      <c r="I4" s="2">
+        <v>40</v>
+      </c>
+      <c r="J4" s="2">
+        <v>40</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0</v>
+      </c>
+      <c r="L4" s="2">
         <v>39</v>
       </c>
-      <c r="M4" s="3">
-        <v>40</v>
-      </c>
-      <c r="N4" s="3">
-        <v>40</v>
-      </c>
-      <c r="O4" s="3"/>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="8"/>
-      <c r="AB4" s="3"/>
-      <c r="AC4" s="3"/>
+      <c r="M4" s="2">
+        <v>15</v>
+      </c>
+      <c r="N4" s="2">
+        <v>40</v>
+      </c>
+      <c r="O4" s="2"/>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="2"/>
+      <c r="AA4" s="7"/>
+      <c r="AB4" s="2"/>
+      <c r="AC4" s="2"/>
       <c r="AF4" s="1"/>
       <c r="AG4" s="1">
         <f t="shared" si="0"/>
@@ -1390,10 +1396,10 @@
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="10">
         <v>200</v>
       </c>
       <c r="D5" s="1">
@@ -1406,9 +1412,11 @@
         <v>200</v>
       </c>
       <c r="G5" s="1">
-        <v>0</v>
-      </c>
-      <c r="H5" s="1"/>
+        <v>200</v>
+      </c>
+      <c r="H5" s="1">
+        <v>200</v>
+      </c>
       <c r="I5" s="1">
         <v>200</v>
       </c>
@@ -1430,22 +1438,22 @@
       <c r="O5" s="1">
         <v>200</v>
       </c>
-      <c r="P5" s="11">
-        <v>200</v>
-      </c>
-      <c r="Q5" s="5">
-        <v>200</v>
-      </c>
-      <c r="R5" s="5">
+      <c r="P5" s="10">
+        <v>200</v>
+      </c>
+      <c r="Q5" s="4">
+        <v>200</v>
+      </c>
+      <c r="R5" s="4">
         <v>193</v>
       </c>
-      <c r="S5" s="7">
+      <c r="S5" s="6">
         <v>199</v>
       </c>
-      <c r="T5" s="5">
-        <v>200</v>
-      </c>
-      <c r="U5" s="5">
+      <c r="T5" s="4">
+        <v>200</v>
+      </c>
+      <c r="U5" s="4">
         <v>200</v>
       </c>
       <c r="V5" s="1">
@@ -1461,7 +1469,7 @@
       <c r="Z5" s="1">
         <v>200</v>
       </c>
-      <c r="AA5" s="7">
+      <c r="AA5" s="6">
         <v>200</v>
       </c>
       <c r="AB5" s="1">
@@ -1481,14 +1489,14 @@
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="10">
         <v>200</v>
       </c>
       <c r="D6" s="1">
-        <v>200</v>
+        <v>27</v>
       </c>
       <c r="E6" s="1">
         <v>200</v>
@@ -1499,7 +1507,9 @@
       <c r="G6" s="1">
         <v>0</v>
       </c>
-      <c r="H6" s="1"/>
+      <c r="H6" s="1">
+        <v>200</v>
+      </c>
       <c r="I6" s="1">
         <v>200</v>
       </c>
@@ -1513,24 +1523,24 @@
         <v>200</v>
       </c>
       <c r="M6" s="1">
-        <v>200</v>
+        <v>106</v>
       </c>
       <c r="N6" s="1">
         <v>200</v>
       </c>
       <c r="O6" s="1"/>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="5"/>
-      <c r="S6" s="7"/>
-      <c r="T6" s="5"/>
-      <c r="U6" s="5"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="4"/>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
       <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
-      <c r="AA6" s="7"/>
+      <c r="AA6" s="6"/>
       <c r="AB6" s="1"/>
       <c r="AC6" s="1"/>
       <c r="AF6" s="1"/>
@@ -1543,65 +1553,67 @@
       </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3" t="s">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="9">
-        <v>200</v>
-      </c>
-      <c r="D7" s="3">
-        <v>200</v>
-      </c>
-      <c r="E7" s="3">
-        <v>200</v>
-      </c>
-      <c r="F7" s="3">
-        <v>0</v>
-      </c>
-      <c r="G7" s="3">
-        <v>0</v>
-      </c>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3">
-        <v>200</v>
-      </c>
-      <c r="J7" s="3">
-        <v>200</v>
-      </c>
-      <c r="K7" s="3">
-        <v>200</v>
-      </c>
-      <c r="L7" s="3">
-        <v>200</v>
-      </c>
-      <c r="M7" s="3">
-        <v>200</v>
-      </c>
-      <c r="N7" s="3">
-        <v>200</v>
-      </c>
-      <c r="O7" s="3"/>
-      <c r="P7" s="9"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="3"/>
-      <c r="S7" s="8"/>
-      <c r="T7" s="3"/>
-      <c r="U7" s="3"/>
-      <c r="V7" s="3"/>
-      <c r="W7" s="3"/>
-      <c r="X7" s="3"/>
-      <c r="Y7" s="3"/>
-      <c r="Z7" s="3"/>
-      <c r="AA7" s="8"/>
-      <c r="AB7" s="3"/>
-      <c r="AC7" s="3"/>
+      <c r="C7" s="8">
+        <v>200</v>
+      </c>
+      <c r="D7" s="2">
+        <v>200</v>
+      </c>
+      <c r="E7" s="2">
+        <v>200</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2">
+        <v>200</v>
+      </c>
+      <c r="I7" s="2">
+        <v>200</v>
+      </c>
+      <c r="J7" s="2">
+        <v>200</v>
+      </c>
+      <c r="K7" s="2">
+        <v>200</v>
+      </c>
+      <c r="L7" s="2">
+        <v>200</v>
+      </c>
+      <c r="M7" s="2">
+        <v>199</v>
+      </c>
+      <c r="N7" s="2">
+        <v>200</v>
+      </c>
+      <c r="O7" s="2"/>
+      <c r="P7" s="8"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="2"/>
+      <c r="Z7" s="2"/>
+      <c r="AA7" s="7"/>
+      <c r="AB7" s="2"/>
+      <c r="AC7" s="2"/>
       <c r="AF7" s="1"/>
       <c r="AG7" s="1">
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
-      <c r="AH7" s="2">
+      <c r="AH7" s="11">
         <v>2.3069444444444445</v>
       </c>
     </row>
@@ -1609,10 +1621,10 @@
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="10">
         <v>24</v>
       </c>
       <c r="D8" s="1">
@@ -1627,7 +1639,9 @@
       <c r="G8" s="1">
         <v>0</v>
       </c>
-      <c r="H8" s="1"/>
+      <c r="H8" s="1">
+        <v>3</v>
+      </c>
       <c r="I8" s="1">
         <v>17</v>
       </c>
@@ -1641,7 +1655,7 @@
         <v>0</v>
       </c>
       <c r="M8" s="1">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="N8" s="1">
         <v>27</v>
@@ -1649,22 +1663,22 @@
       <c r="O8" s="1">
         <v>21</v>
       </c>
-      <c r="P8" s="11">
+      <c r="P8" s="10">
         <v>5</v>
       </c>
-      <c r="Q8" s="5">
+      <c r="Q8" s="4">
         <v>16</v>
       </c>
-      <c r="R8" s="5">
+      <c r="R8" s="4">
         <v>13</v>
       </c>
-      <c r="S8" s="7">
+      <c r="S8" s="6">
         <v>12</v>
       </c>
-      <c r="T8" s="5">
+      <c r="T8" s="4">
         <v>20</v>
       </c>
-      <c r="U8" s="5">
+      <c r="U8" s="4">
         <v>12</v>
       </c>
       <c r="V8" s="1">
@@ -1682,7 +1696,7 @@
       <c r="Z8" s="1">
         <v>12</v>
       </c>
-      <c r="AA8" s="7">
+      <c r="AA8" s="6">
         <v>18</v>
       </c>
       <c r="AB8" s="1">
@@ -1700,14 +1714,14 @@
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="10">
         <v>24</v>
       </c>
       <c r="D9" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E9" s="1">
         <v>2</v>
@@ -1718,7 +1732,9 @@
       <c r="G9" s="1">
         <v>0</v>
       </c>
-      <c r="H9" s="1"/>
+      <c r="H9" s="1">
+        <v>5</v>
+      </c>
       <c r="I9" s="1">
         <v>21</v>
       </c>
@@ -1732,24 +1748,24 @@
         <v>17</v>
       </c>
       <c r="M9" s="1">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="N9" s="1">
         <v>26</v>
       </c>
       <c r="O9" s="1"/>
-      <c r="P9" s="11"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="7"/>
-      <c r="T9" s="5"/>
-      <c r="U9" s="5"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="4"/>
       <c r="V9" s="1"/>
       <c r="W9" s="1"/>
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
-      <c r="AA9" s="7"/>
+      <c r="AA9" s="6"/>
       <c r="AB9" s="1"/>
       <c r="AC9" s="1"/>
       <c r="AF9" s="1"/>
@@ -1760,59 +1776,61 @@
       <c r="AH9" s="1"/>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3" t="s">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="8">
         <v>11</v>
       </c>
-      <c r="D10" s="3">
-        <v>0</v>
-      </c>
-      <c r="E10" s="3">
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2">
         <v>9</v>
       </c>
-      <c r="F10" s="3">
-        <v>0</v>
-      </c>
-      <c r="G10" s="3">
-        <v>0</v>
-      </c>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3">
+      <c r="F10" s="2">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0</v>
+      </c>
+      <c r="H10" s="2">
+        <v>4</v>
+      </c>
+      <c r="I10" s="2">
         <v>8</v>
       </c>
-      <c r="J10" s="3">
-        <v>8</v>
-      </c>
-      <c r="K10" s="3">
+      <c r="J10" s="2">
+        <v>6</v>
+      </c>
+      <c r="K10" s="2">
         <v>14</v>
       </c>
-      <c r="L10" s="3">
+      <c r="L10" s="2">
         <v>6</v>
       </c>
-      <c r="M10" s="3">
+      <c r="M10" s="2">
+        <v>5</v>
+      </c>
+      <c r="N10" s="2">
         <v>18</v>
       </c>
-      <c r="N10" s="3">
-        <v>18</v>
-      </c>
-      <c r="O10" s="3"/>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="3"/>
-      <c r="R10" s="3"/>
-      <c r="S10" s="8"/>
-      <c r="T10" s="3"/>
-      <c r="U10" s="3"/>
-      <c r="V10" s="3"/>
-      <c r="W10" s="3"/>
-      <c r="X10" s="3"/>
-      <c r="Y10" s="3"/>
-      <c r="Z10" s="3"/>
-      <c r="AA10" s="8"/>
-      <c r="AB10" s="3"/>
-      <c r="AC10" s="3"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="2"/>
+      <c r="Z10" s="2"/>
+      <c r="AA10" s="7"/>
+      <c r="AB10" s="2"/>
+      <c r="AC10" s="2"/>
       <c r="AF10" s="1"/>
       <c r="AG10" s="1">
         <f t="shared" si="0"/>
@@ -1824,10 +1842,10 @@
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="10">
         <v>946</v>
       </c>
       <c r="D11" s="1">
@@ -1837,12 +1855,14 @@
         <v>568</v>
       </c>
       <c r="F11" s="1">
-        <v>217</v>
+        <v>298</v>
       </c>
       <c r="G11" s="1">
         <v>0</v>
       </c>
-      <c r="H11" s="1"/>
+      <c r="H11" s="1">
+        <v>543</v>
+      </c>
       <c r="I11" s="1">
         <v>935</v>
       </c>
@@ -1850,13 +1870,13 @@
         <v>965</v>
       </c>
       <c r="K11" s="1">
-        <v>779</v>
+        <v>925</v>
       </c>
       <c r="L11" s="1">
         <v>0</v>
       </c>
       <c r="M11" s="1">
-        <v>801</v>
+        <v>564</v>
       </c>
       <c r="N11" s="1">
         <v>806</v>
@@ -1864,22 +1884,22 @@
       <c r="O11" s="1">
         <v>967</v>
       </c>
-      <c r="P11" s="11">
+      <c r="P11" s="10">
         <v>947</v>
       </c>
-      <c r="Q11" s="5">
+      <c r="Q11" s="4">
         <v>937</v>
       </c>
-      <c r="R11" s="5">
+      <c r="R11" s="4">
         <v>869</v>
       </c>
-      <c r="S11" s="7">
+      <c r="S11" s="6">
         <v>830</v>
       </c>
-      <c r="T11" s="5">
+      <c r="T11" s="4">
         <v>988</v>
       </c>
-      <c r="U11" s="5">
+      <c r="U11" s="4">
         <v>958</v>
       </c>
       <c r="V11" s="1">
@@ -1897,7 +1917,7 @@
       <c r="Z11" s="1">
         <v>918</v>
       </c>
-      <c r="AA11" s="7">
+      <c r="AA11" s="6">
         <v>964</v>
       </c>
       <c r="AB11" s="1">
@@ -1915,119 +1935,123 @@
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="10">
         <v>964</v>
       </c>
       <c r="D12" s="1">
-        <v>460</v>
+        <v>536</v>
       </c>
       <c r="E12" s="1">
         <v>151</v>
       </c>
       <c r="F12" s="1">
-        <v>298</v>
+        <v>0</v>
       </c>
       <c r="G12" s="1">
         <v>0</v>
       </c>
-      <c r="H12" s="1"/>
+      <c r="H12" s="1">
+        <v>422</v>
+      </c>
       <c r="I12" s="1">
         <v>941</v>
       </c>
       <c r="J12" s="1">
-        <v>807</v>
+        <v>965</v>
       </c>
       <c r="K12" s="1">
-        <v>569</v>
+        <v>654</v>
       </c>
       <c r="L12" s="1">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="M12" s="1">
-        <v>806</v>
+        <v>431</v>
       </c>
       <c r="N12" s="1">
         <v>813</v>
       </c>
       <c r="O12" s="1"/>
-      <c r="P12" s="11"/>
-      <c r="Q12" s="5"/>
-      <c r="R12" s="5"/>
-      <c r="S12" s="7"/>
-      <c r="T12" s="5"/>
-      <c r="U12" s="5"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="4"/>
+      <c r="U12" s="4"/>
       <c r="V12" s="1"/>
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
-      <c r="AA12" s="7"/>
+      <c r="AA12" s="6"/>
       <c r="AB12" s="1"/>
       <c r="AC12" s="1"/>
       <c r="AF12" s="1"/>
       <c r="AG12" s="1">
         <f t="shared" si="0"/>
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="AH12" s="1"/>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3" t="s">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="8">
         <v>914</v>
       </c>
-      <c r="D13" s="3">
-        <v>0</v>
-      </c>
-      <c r="E13" s="3">
+      <c r="D13" s="2">
+        <v>53</v>
+      </c>
+      <c r="E13" s="2">
         <v>422</v>
       </c>
-      <c r="F13" s="3">
-        <v>0</v>
-      </c>
-      <c r="G13" s="3">
-        <v>0</v>
-      </c>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3">
+      <c r="F13" s="2">
+        <v>0</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0</v>
+      </c>
+      <c r="H13" s="2">
+        <v>97</v>
+      </c>
+      <c r="I13" s="2">
         <v>613</v>
       </c>
-      <c r="J13" s="3">
-        <v>453</v>
-      </c>
-      <c r="K13" s="3">
-        <v>159</v>
-      </c>
-      <c r="L13" s="3">
-        <v>481</v>
-      </c>
-      <c r="M13" s="3">
-        <v>787</v>
-      </c>
-      <c r="N13" s="3">
+      <c r="J13" s="2">
+        <v>512</v>
+      </c>
+      <c r="K13" s="2">
+        <v>189</v>
+      </c>
+      <c r="L13" s="2">
+        <v>482</v>
+      </c>
+      <c r="M13" s="2">
+        <v>224</v>
+      </c>
+      <c r="N13" s="2">
         <v>795</v>
       </c>
-      <c r="O13" s="3"/>
-      <c r="P13" s="9"/>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="3"/>
-      <c r="S13" s="8"/>
-      <c r="T13" s="3"/>
-      <c r="U13" s="3"/>
-      <c r="V13" s="3"/>
-      <c r="W13" s="3"/>
-      <c r="X13" s="3"/>
-      <c r="Y13" s="3"/>
-      <c r="Z13" s="3"/>
-      <c r="AA13" s="8"/>
-      <c r="AB13" s="3"/>
-      <c r="AC13" s="3"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="7"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2"/>
+      <c r="Y13" s="2"/>
+      <c r="Z13" s="2"/>
+      <c r="AA13" s="7"/>
+      <c r="AB13" s="2"/>
+      <c r="AC13" s="2"/>
       <c r="AF13" s="1"/>
       <c r="AG13" s="1">
         <f t="shared" si="0"/>
@@ -2039,10 +2063,10 @@
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="11">
+      <c r="C14" s="10">
         <v>639</v>
       </c>
       <c r="D14" s="1">
@@ -2052,17 +2076,19 @@
         <v>0</v>
       </c>
       <c r="F14" s="1">
-        <v>88</v>
+        <v>162</v>
       </c>
       <c r="G14" s="1">
         <v>0</v>
       </c>
-      <c r="H14" s="1"/>
+      <c r="H14" s="1">
+        <v>5</v>
+      </c>
       <c r="I14" s="1">
         <v>411</v>
       </c>
       <c r="J14" s="1">
-        <v>541</v>
+        <v>608</v>
       </c>
       <c r="K14" s="1">
         <v>0</v>
@@ -2071,28 +2097,28 @@
         <v>0</v>
       </c>
       <c r="M14" s="1">
-        <v>553</v>
+        <v>390</v>
       </c>
       <c r="N14" s="1"/>
       <c r="O14" s="1">
         <v>497</v>
       </c>
-      <c r="P14" s="11">
+      <c r="P14" s="10">
         <v>927</v>
       </c>
-      <c r="Q14" s="5">
+      <c r="Q14" s="4">
         <v>445</v>
       </c>
-      <c r="R14" s="5">
+      <c r="R14" s="4">
         <v>633</v>
       </c>
-      <c r="S14" s="7">
+      <c r="S14" s="6">
         <v>263</v>
       </c>
-      <c r="T14" s="5">
+      <c r="T14" s="4">
         <v>938</v>
       </c>
-      <c r="U14" s="5">
+      <c r="U14" s="4">
         <v>967</v>
       </c>
       <c r="V14" s="1">
@@ -2110,7 +2136,7 @@
       <c r="Z14" s="1">
         <v>929</v>
       </c>
-      <c r="AA14" s="7">
+      <c r="AA14" s="6">
         <v>799</v>
       </c>
       <c r="AB14" s="1">
@@ -2128,10 +2154,10 @@
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="11">
+      <c r="C15" s="10">
         <v>872</v>
       </c>
       <c r="D15" s="1">
@@ -2146,12 +2172,14 @@
       <c r="G15" s="1">
         <v>0</v>
       </c>
-      <c r="H15" s="1"/>
+      <c r="H15" s="1">
+        <v>0</v>
+      </c>
       <c r="I15" s="1">
         <v>401</v>
       </c>
       <c r="J15" s="1">
-        <v>611</v>
+        <v>448</v>
       </c>
       <c r="K15" s="1">
         <v>0</v>
@@ -2160,22 +2188,22 @@
         <v>939</v>
       </c>
       <c r="M15" s="1">
-        <v>768</v>
+        <v>230</v>
       </c>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
-      <c r="P15" s="11"/>
-      <c r="Q15" s="5"/>
-      <c r="R15" s="5"/>
-      <c r="S15" s="7"/>
-      <c r="T15" s="5"/>
-      <c r="U15" s="5"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="4"/>
+      <c r="S15" s="6"/>
+      <c r="T15" s="4"/>
+      <c r="U15" s="4"/>
       <c r="V15" s="1"/>
       <c r="W15" s="1"/>
       <c r="X15" s="1"/>
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
-      <c r="AA15" s="7"/>
+      <c r="AA15" s="6"/>
       <c r="AB15" s="1"/>
       <c r="AC15" s="1"/>
       <c r="AD15" s="1"/>
@@ -2186,14 +2214,14 @@
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C16" s="10">
         <v>958</v>
       </c>
       <c r="D16" s="1">
-        <v>56</v>
+        <v>209</v>
       </c>
       <c r="E16" s="1">
         <v>74</v>
@@ -2204,36 +2232,38 @@
       <c r="G16" s="1">
         <v>0</v>
       </c>
-      <c r="H16" s="1"/>
+      <c r="H16" s="1">
+        <v>254</v>
+      </c>
       <c r="I16" s="1">
         <v>946</v>
       </c>
       <c r="J16" s="1">
-        <v>805</v>
+        <v>956</v>
       </c>
       <c r="K16" s="1">
         <v>0</v>
       </c>
       <c r="L16" s="1">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="M16" s="1">
-        <v>806</v>
+        <v>392</v>
       </c>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
-      <c r="P16" s="11"/>
-      <c r="Q16" s="5"/>
-      <c r="R16" s="5"/>
-      <c r="S16" s="7"/>
-      <c r="T16" s="5"/>
-      <c r="U16" s="5"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="4"/>
+      <c r="R16" s="4"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="4"/>
+      <c r="U16" s="4"/>
       <c r="V16" s="1"/>
       <c r="W16" s="1"/>
       <c r="X16" s="1"/>
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
-      <c r="AA16" s="7"/>
+      <c r="AA16" s="6"/>
       <c r="AB16" s="1"/>
       <c r="AC16" s="1"/>
       <c r="AD16" s="1"/>
@@ -2352,6 +2382,246 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2">
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3">
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G4">
+    <cfRule type="colorScale" priority="30">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G5">
+    <cfRule type="colorScale" priority="31">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G6">
+    <cfRule type="colorScale" priority="32">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G7">
+    <cfRule type="colorScale" priority="33">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G8">
+    <cfRule type="colorScale" priority="34">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G9">
+    <cfRule type="colorScale" priority="35">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G10">
+    <cfRule type="colorScale" priority="36">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G11">
+    <cfRule type="colorScale" priority="37">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G12">
+    <cfRule type="colorScale" priority="38">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G13">
+    <cfRule type="colorScale" priority="39">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G14">
+    <cfRule type="colorScale" priority="40">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G15">
+    <cfRule type="colorScale" priority="41">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G16">
+    <cfRule type="colorScale" priority="42">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:J2">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3:J3">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4:J4">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I5:J5">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I6:J6">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I7:J7">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
@@ -2363,7 +2633,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3">
+  <conditionalFormatting sqref="I8:J8">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -2375,7 +2645,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G4">
+  <conditionalFormatting sqref="I9:J9">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
@@ -2387,7 +2657,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G5">
+  <conditionalFormatting sqref="I10:J10">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
@@ -2399,7 +2669,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G6">
+  <conditionalFormatting sqref="I11:J11">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
@@ -2411,7 +2681,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G7">
+  <conditionalFormatting sqref="I12:J12">
     <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
@@ -2423,7 +2693,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G8">
+  <conditionalFormatting sqref="I13:J13">
     <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
@@ -2435,7 +2705,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G9">
+  <conditionalFormatting sqref="I14:J14">
     <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
@@ -2447,7 +2717,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G10">
+  <conditionalFormatting sqref="I15:J15">
     <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
@@ -2459,7 +2729,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G11">
+  <conditionalFormatting sqref="I16:J16">
     <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
@@ -2471,67 +2741,295 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G12">
-    <cfRule type="colorScale" priority="28">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G13">
-    <cfRule type="colorScale" priority="29">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G14">
-    <cfRule type="colorScale" priority="30">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G15">
-    <cfRule type="colorScale" priority="31">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G16">
-    <cfRule type="colorScale" priority="32">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I2:J2">
+  <conditionalFormatting sqref="K15">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K16">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:F2 H2 L2:N2">
+    <cfRule type="colorScale" priority="77">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:F3 H3 L3:N3">
+    <cfRule type="colorScale" priority="81">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C4:F4 H4 L4:N4">
+    <cfRule type="colorScale" priority="85">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5:F5 H5 L5:N5">
+    <cfRule type="colorScale" priority="89">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C6:F6 H6 L6:N6">
+    <cfRule type="colorScale" priority="93">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C7:F7 H7 L7:N7">
+    <cfRule type="colorScale" priority="97">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8:F8 H8 L8:N8">
+    <cfRule type="colorScale" priority="101">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9:F9 H9 L9:N9">
+    <cfRule type="colorScale" priority="105">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10:F10 H10 L10:N10">
+    <cfRule type="colorScale" priority="109">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11:F11 H11 L11:N11">
+    <cfRule type="colorScale" priority="113">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12:F12 H12 L12:N12">
+    <cfRule type="colorScale" priority="117">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13:F13 H13 L13:N13">
+    <cfRule type="colorScale" priority="121">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14:F14 H14 L14:N14">
+    <cfRule type="colorScale" priority="125">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15:F15 H15 L15:N15">
+    <cfRule type="colorScale" priority="134">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C16:F16 H16 L16:N16">
+    <cfRule type="colorScale" priority="137">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:N4">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5:N7">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8:N10">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11:N13">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14:N16">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P2:AA2">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P5:AA5">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P8:AA8">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -2543,368 +3041,20 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3:J3">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I4:J4">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I5:J5">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I6:J6">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I7:J7">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I8:J8">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I9:J9">
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I10:J10">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I11:J11">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I12:J12">
-    <cfRule type="colorScale" priority="13">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I13:J13">
-    <cfRule type="colorScale" priority="14">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I14:J14">
-    <cfRule type="colorScale" priority="15">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I15:J15">
-    <cfRule type="colorScale" priority="16">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I16:J16">
-    <cfRule type="colorScale" priority="17">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K15">
+  <conditionalFormatting sqref="P11:AA11">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P14:AA14">
     <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K16">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2:F2 H2 L2:N2">
-    <cfRule type="colorScale" priority="67">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C3:F3 H3 L3:N3">
-    <cfRule type="colorScale" priority="71">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C4:F4 H4 L4:N4">
-    <cfRule type="colorScale" priority="75">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C5:F5 H5 L5:N5">
-    <cfRule type="colorScale" priority="79">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C6:F6 H6 L6:N6">
-    <cfRule type="colorScale" priority="83">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C7:F7 H7 L7:N7">
-    <cfRule type="colorScale" priority="87">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C8:F8 H8 L8:N8">
-    <cfRule type="colorScale" priority="91">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C9:F9 H9 L9:N9">
-    <cfRule type="colorScale" priority="95">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C10:F10 H10 L10:N10">
-    <cfRule type="colorScale" priority="99">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C11:F11 H11 L11:N11">
-    <cfRule type="colorScale" priority="103">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C12:F12 H12 L12:N12">
-    <cfRule type="colorScale" priority="107">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C13:F13 H13 L13:N13">
-    <cfRule type="colorScale" priority="111">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C14:F14 H14 L14:N14">
-    <cfRule type="colorScale" priority="115">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C15:F15 H15 L15:N15">
-    <cfRule type="colorScale" priority="124">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C16:F16 H16 L16:N16">
-    <cfRule type="colorScale" priority="127">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>

<commit_message>
Results section has all content, potentially a rough draft
</commit_message>
<xml_diff>
--- a/tncData.xlsx
+++ b/tncData.xlsx
@@ -1056,10 +1056,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH19"/>
+  <dimension ref="A1:AH31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="R28" sqref="R28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2293,7 +2293,10 @@
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
-      <c r="U17" s="1"/>
+      <c r="U17" s="1">
+        <f>AVERAGE(P2:AA2)</f>
+        <v>39.916666666666664</v>
+      </c>
       <c r="V17" s="1"/>
       <c r="W17" s="1"/>
       <c r="X17" s="1"/>
@@ -2380,6 +2383,54 @@
       <c r="AG19" s="1"/>
       <c r="AH19" s="1"/>
     </row>
+    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="U20" s="1">
+        <f t="shared" ref="U18:U31" si="1">AVERAGE(P5:AA5)</f>
+        <v>199.27272727272728</v>
+      </c>
+    </row>
+    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="U21" s="1"/>
+    </row>
+    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="U22" s="1"/>
+    </row>
+    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="U23" s="1">
+        <f t="shared" si="1"/>
+        <v>14.583333333333334</v>
+      </c>
+    </row>
+    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="U24" s="1"/>
+    </row>
+    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="U25" s="1"/>
+    </row>
+    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="U26" s="1">
+        <f t="shared" si="1"/>
+        <v>935.08333333333337</v>
+      </c>
+    </row>
+    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="U27" s="1"/>
+    </row>
+    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="U28" s="1"/>
+    </row>
+    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="U29" s="1">
+        <f t="shared" si="1"/>
+        <v>777.91666666666663</v>
+      </c>
+    </row>
+    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="U30" s="1"/>
+    </row>
+    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="U31" s="1"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="G2">
     <cfRule type="colorScale" priority="28">

</xml_diff>

<commit_message>
Full draft of defense presentation
</commit_message>
<xml_diff>
--- a/tncData.xlsx
+++ b/tncData.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robbie\gitDir\rrxthesis\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="12180"/>
   </bookViews>
   <sheets>
     <sheet name="tncData" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
   <si>
     <t>.wav file</t>
   </si>
@@ -137,6 +131,10 @@
   </si>
   <si>
     <t>Goertzel (100%)</t>
+  </si>
+  <si>
+    <t>AVERAGE
+HARDWARE</t>
   </si>
 </sst>
 </file>
@@ -460,7 +458,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -655,6 +653,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -700,7 +735,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -733,6 +768,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1048,7 +1092,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1056,20 +1100,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH31"/>
+  <dimension ref="A1:AI31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="R28" sqref="R28"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:AB16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.140625" customWidth="1"/>
     <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="34" width="11.5703125" customWidth="1"/>
+    <col min="3" max="35" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1115,57 +1159,60 @@
       <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="P1" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="T1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="AA1" s="7" t="s">
+      <c r="AB1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="AF1" s="1"/>
-      <c r="AG1" s="1" t="s">
+      <c r="AG1" s="1"/>
+      <c r="AH1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
@@ -1211,19 +1258,20 @@
       <c r="O2" s="3">
         <v>40</v>
       </c>
-      <c r="P2" s="9">
-        <v>40</v>
-      </c>
-      <c r="Q2" s="3">
+      <c r="P2" s="13">
+        <f>AVERAGE(Q2:AB2)</f>
+        <v>39.916666666666664</v>
+      </c>
+      <c r="Q2" s="9">
         <v>40</v>
       </c>
       <c r="R2" s="3">
+        <v>40</v>
+      </c>
+      <c r="S2" s="3">
         <v>39</v>
       </c>
-      <c r="S2" s="5">
-        <v>40</v>
-      </c>
-      <c r="T2" s="3">
+      <c r="T2" s="5">
         <v>40</v>
       </c>
       <c r="U2" s="3">
@@ -1244,25 +1292,28 @@
       <c r="Z2" s="3">
         <v>40</v>
       </c>
-      <c r="AA2" s="5">
-        <v>40</v>
-      </c>
-      <c r="AB2" s="3">
+      <c r="AA2" s="3">
+        <v>40</v>
+      </c>
+      <c r="AB2" s="5">
         <v>40</v>
       </c>
       <c r="AC2" s="3">
         <v>40</v>
       </c>
-      <c r="AF2" s="1"/>
-      <c r="AG2" s="1">
-        <f>MAX(C2:AF2)</f>
-        <v>40</v>
-      </c>
+      <c r="AD2" s="3">
+        <v>40</v>
+      </c>
+      <c r="AG2" s="1"/>
       <c r="AH2" s="1">
+        <f>MAX(C2:AG2)</f>
+        <v>40</v>
+      </c>
+      <c r="AI2" s="1">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4" t="s">
         <v>23</v>
@@ -1304,30 +1355,31 @@
         <v>40</v>
       </c>
       <c r="O3" s="4"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="4"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="10"/>
       <c r="R3" s="4"/>
-      <c r="S3" s="6"/>
-      <c r="T3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="6"/>
       <c r="U3" s="4"/>
       <c r="V3" s="4"/>
       <c r="W3" s="4"/>
       <c r="X3" s="4"/>
       <c r="Y3" s="4"/>
       <c r="Z3" s="4"/>
-      <c r="AA3" s="6"/>
-      <c r="AB3" s="4"/>
+      <c r="AA3" s="4"/>
+      <c r="AB3" s="6"/>
       <c r="AC3" s="4"/>
-      <c r="AF3" s="1"/>
-      <c r="AG3" s="1">
-        <f t="shared" ref="AG3:AG14" si="0">MAX(C3:AF3)</f>
-        <v>40</v>
-      </c>
+      <c r="AD3" s="4"/>
+      <c r="AG3" s="1"/>
       <c r="AH3" s="1">
+        <f t="shared" ref="AH3:AH14" si="0">MAX(C3:AG3)</f>
+        <v>40</v>
+      </c>
+      <c r="AI3" s="1">
         <v>184</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
         <v>24</v>
@@ -1369,30 +1421,31 @@
         <v>40</v>
       </c>
       <c r="O4" s="2"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="2"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="8"/>
       <c r="R4" s="2"/>
-      <c r="S4" s="7"/>
-      <c r="T4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="7"/>
       <c r="U4" s="2"/>
       <c r="V4" s="2"/>
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
       <c r="Z4" s="2"/>
-      <c r="AA4" s="7"/>
-      <c r="AB4" s="2"/>
+      <c r="AA4" s="2"/>
+      <c r="AB4" s="7"/>
       <c r="AC4" s="2"/>
-      <c r="AF4" s="1"/>
-      <c r="AG4" s="1">
+      <c r="AD4" s="2"/>
+      <c r="AG4" s="1"/>
+      <c r="AH4" s="1">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="AH4" s="1">
+      <c r="AI4" s="1">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -1438,25 +1491,26 @@
       <c r="O5" s="1">
         <v>200</v>
       </c>
-      <c r="P5" s="10">
-        <v>200</v>
-      </c>
-      <c r="Q5" s="4">
+      <c r="P5" s="13">
+        <f>AVERAGE(Q5:AB5)</f>
+        <v>199.27272727272728</v>
+      </c>
+      <c r="Q5" s="10">
         <v>200</v>
       </c>
       <c r="R5" s="4">
+        <v>200</v>
+      </c>
+      <c r="S5" s="4">
         <v>193</v>
       </c>
-      <c r="S5" s="6">
+      <c r="T5" s="6">
         <v>199</v>
       </c>
-      <c r="T5" s="4">
-        <v>200</v>
-      </c>
       <c r="U5" s="4">
         <v>200</v>
       </c>
-      <c r="V5" s="1">
+      <c r="V5" s="4">
         <v>200</v>
       </c>
       <c r="W5" s="1">
@@ -1465,29 +1519,32 @@
       <c r="X5" s="1">
         <v>200</v>
       </c>
-      <c r="Y5" s="1"/>
-      <c r="Z5" s="1">
-        <v>200</v>
-      </c>
-      <c r="AA5" s="6">
-        <v>200</v>
-      </c>
-      <c r="AB5" s="1">
+      <c r="Y5" s="1">
+        <v>200</v>
+      </c>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="1">
+        <v>200</v>
+      </c>
+      <c r="AB5" s="6">
         <v>200</v>
       </c>
       <c r="AC5" s="1">
         <v>200</v>
       </c>
-      <c r="AF5" s="1"/>
-      <c r="AG5" s="1">
+      <c r="AD5" s="1">
+        <v>200</v>
+      </c>
+      <c r="AG5" s="1"/>
+      <c r="AH5" s="1">
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
-      <c r="AH5" s="1">
+      <c r="AI5" s="1">
         <v>1549</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="4" t="s">
         <v>23</v>
@@ -1529,30 +1586,31 @@
         <v>200</v>
       </c>
       <c r="O6" s="1"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="4"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="10"/>
       <c r="R6" s="4"/>
-      <c r="S6" s="6"/>
-      <c r="T6" s="4"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="6"/>
       <c r="U6" s="4"/>
-      <c r="V6" s="1"/>
+      <c r="V6" s="4"/>
       <c r="W6" s="1"/>
       <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
-      <c r="AA6" s="6"/>
-      <c r="AB6" s="1"/>
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="6"/>
       <c r="AC6" s="1"/>
-      <c r="AF6" s="1"/>
-      <c r="AG6" s="1">
+      <c r="AD6" s="1"/>
+      <c r="AG6" s="1"/>
+      <c r="AH6" s="1">
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
-      <c r="AH6" s="1">
+      <c r="AI6" s="1">
         <v>1549</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
         <v>24</v>
@@ -1594,30 +1652,31 @@
         <v>200</v>
       </c>
       <c r="O7" s="2"/>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="2"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="8"/>
       <c r="R7" s="2"/>
-      <c r="S7" s="7"/>
-      <c r="T7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="7"/>
       <c r="U7" s="2"/>
       <c r="V7" s="2"/>
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
       <c r="Y7" s="2"/>
       <c r="Z7" s="2"/>
-      <c r="AA7" s="7"/>
-      <c r="AB7" s="2"/>
+      <c r="AA7" s="2"/>
+      <c r="AB7" s="7"/>
       <c r="AC7" s="2"/>
-      <c r="AF7" s="1"/>
-      <c r="AG7" s="1">
+      <c r="AD7" s="2"/>
+      <c r="AG7" s="1"/>
+      <c r="AH7" s="1">
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
-      <c r="AH7" s="11">
+      <c r="AI7" s="11">
         <v>2.3069444444444445</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -1663,56 +1722,60 @@
       <c r="O8" s="1">
         <v>21</v>
       </c>
-      <c r="P8" s="10">
+      <c r="P8" s="13">
+        <f>AVERAGE(Q8:AB8)</f>
+        <v>14.583333333333334</v>
+      </c>
+      <c r="Q8" s="10">
         <v>5</v>
       </c>
-      <c r="Q8" s="4">
+      <c r="R8" s="4">
         <v>16</v>
       </c>
-      <c r="R8" s="4">
+      <c r="S8" s="4">
         <v>13</v>
       </c>
-      <c r="S8" s="6">
+      <c r="T8" s="6">
         <v>12</v>
       </c>
-      <c r="T8" s="4">
+      <c r="U8" s="4">
         <v>20</v>
       </c>
-      <c r="U8" s="4">
+      <c r="V8" s="4">
         <v>12</v>
       </c>
-      <c r="V8" s="1">
+      <c r="W8" s="1">
         <v>12</v>
       </c>
-      <c r="W8" s="1">
+      <c r="X8" s="1">
         <v>5</v>
-      </c>
-      <c r="X8" s="1">
-        <v>25</v>
       </c>
       <c r="Y8" s="1">
         <v>25</v>
       </c>
       <c r="Z8" s="1">
+        <v>25</v>
+      </c>
+      <c r="AA8" s="1">
         <v>12</v>
       </c>
-      <c r="AA8" s="6">
+      <c r="AB8" s="6">
         <v>18</v>
-      </c>
-      <c r="AB8" s="1">
-        <v>24</v>
       </c>
       <c r="AC8" s="1">
         <v>24</v>
       </c>
-      <c r="AF8" s="1"/>
-      <c r="AG8" s="1">
+      <c r="AD8" s="1">
+        <v>24</v>
+      </c>
+      <c r="AG8" s="1"/>
+      <c r="AH8" s="1">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="AH8" s="1"/>
+      <c r="AI8" s="1"/>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="4" t="s">
         <v>23</v>
@@ -1754,28 +1817,29 @@
         <v>26</v>
       </c>
       <c r="O9" s="1"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="4"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="10"/>
       <c r="R9" s="4"/>
-      <c r="S9" s="6"/>
-      <c r="T9" s="4"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="6"/>
       <c r="U9" s="4"/>
-      <c r="V9" s="1"/>
+      <c r="V9" s="4"/>
       <c r="W9" s="1"/>
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
-      <c r="AA9" s="6"/>
-      <c r="AB9" s="1"/>
+      <c r="AA9" s="1"/>
+      <c r="AB9" s="6"/>
       <c r="AC9" s="1"/>
-      <c r="AF9" s="1"/>
-      <c r="AG9" s="1">
+      <c r="AD9" s="1"/>
+      <c r="AG9" s="1"/>
+      <c r="AH9" s="1">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="AH9" s="1"/>
+      <c r="AI9" s="1"/>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
         <v>24</v>
@@ -1817,28 +1881,29 @@
         <v>18</v>
       </c>
       <c r="O10" s="2"/>
-      <c r="P10" s="8"/>
-      <c r="Q10" s="2"/>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="8"/>
       <c r="R10" s="2"/>
-      <c r="S10" s="7"/>
-      <c r="T10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="7"/>
       <c r="U10" s="2"/>
       <c r="V10" s="2"/>
       <c r="W10" s="2"/>
       <c r="X10" s="2"/>
       <c r="Y10" s="2"/>
       <c r="Z10" s="2"/>
-      <c r="AA10" s="7"/>
-      <c r="AB10" s="2"/>
+      <c r="AA10" s="2"/>
+      <c r="AB10" s="7"/>
       <c r="AC10" s="2"/>
-      <c r="AF10" s="1"/>
-      <c r="AG10" s="1">
+      <c r="AD10" s="2"/>
+      <c r="AG10" s="1"/>
+      <c r="AH10" s="1">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="AH10" s="1"/>
+      <c r="AI10" s="1"/>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
@@ -1884,56 +1949,60 @@
       <c r="O11" s="1">
         <v>967</v>
       </c>
-      <c r="P11" s="10">
+      <c r="P11" s="13">
+        <f>AVERAGE(Q11:AB11)</f>
+        <v>935.08333333333337</v>
+      </c>
+      <c r="Q11" s="10">
         <v>947</v>
       </c>
-      <c r="Q11" s="4">
+      <c r="R11" s="4">
         <v>937</v>
       </c>
-      <c r="R11" s="4">
+      <c r="S11" s="4">
         <v>869</v>
       </c>
-      <c r="S11" s="6">
+      <c r="T11" s="6">
         <v>830</v>
       </c>
-      <c r="T11" s="4">
+      <c r="U11" s="4">
         <v>988</v>
       </c>
-      <c r="U11" s="4">
+      <c r="V11" s="4">
         <v>958</v>
       </c>
-      <c r="V11" s="1">
+      <c r="W11" s="1">
         <v>985</v>
       </c>
-      <c r="W11" s="1">
+      <c r="X11" s="1">
         <v>837</v>
       </c>
-      <c r="X11" s="1">
+      <c r="Y11" s="1">
         <v>981</v>
       </c>
-      <c r="Y11" s="1">
+      <c r="Z11" s="1">
         <v>1007</v>
       </c>
-      <c r="Z11" s="1">
+      <c r="AA11" s="1">
         <v>918</v>
       </c>
-      <c r="AA11" s="6">
+      <c r="AB11" s="6">
         <v>964</v>
-      </c>
-      <c r="AB11" s="1">
-        <v>966</v>
       </c>
       <c r="AC11" s="1">
         <v>966</v>
       </c>
-      <c r="AF11" s="1"/>
-      <c r="AG11" s="1">
+      <c r="AD11" s="1">
+        <v>966</v>
+      </c>
+      <c r="AG11" s="1"/>
+      <c r="AH11" s="1">
         <f t="shared" si="0"/>
         <v>1007</v>
       </c>
-      <c r="AH11" s="1"/>
+      <c r="AI11" s="1"/>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="4" t="s">
         <v>23</v>
@@ -1975,28 +2044,29 @@
         <v>813</v>
       </c>
       <c r="O12" s="1"/>
-      <c r="P12" s="10"/>
-      <c r="Q12" s="4"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="10"/>
       <c r="R12" s="4"/>
-      <c r="S12" s="6"/>
-      <c r="T12" s="4"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="6"/>
       <c r="U12" s="4"/>
-      <c r="V12" s="1"/>
+      <c r="V12" s="4"/>
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
-      <c r="AA12" s="6"/>
-      <c r="AB12" s="1"/>
+      <c r="AA12" s="1"/>
+      <c r="AB12" s="6"/>
       <c r="AC12" s="1"/>
-      <c r="AF12" s="1"/>
-      <c r="AG12" s="1">
+      <c r="AD12" s="1"/>
+      <c r="AG12" s="1"/>
+      <c r="AH12" s="1">
         <f t="shared" si="0"/>
         <v>965</v>
       </c>
-      <c r="AH12" s="1"/>
+      <c r="AI12" s="1"/>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
         <v>24</v>
@@ -2038,28 +2108,29 @@
         <v>795</v>
       </c>
       <c r="O13" s="2"/>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="2"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="8"/>
       <c r="R13" s="2"/>
-      <c r="S13" s="7"/>
-      <c r="T13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="7"/>
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
       <c r="W13" s="2"/>
       <c r="X13" s="2"/>
       <c r="Y13" s="2"/>
       <c r="Z13" s="2"/>
-      <c r="AA13" s="7"/>
-      <c r="AB13" s="2"/>
+      <c r="AA13" s="2"/>
+      <c r="AB13" s="7"/>
       <c r="AC13" s="2"/>
-      <c r="AF13" s="1"/>
-      <c r="AG13" s="1">
+      <c r="AD13" s="2"/>
+      <c r="AG13" s="1"/>
+      <c r="AH13" s="1">
         <f t="shared" si="0"/>
         <v>914</v>
       </c>
-      <c r="AH13" s="1"/>
+      <c r="AI13" s="1"/>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
@@ -2103,56 +2174,60 @@
       <c r="O14" s="1">
         <v>497</v>
       </c>
-      <c r="P14" s="10">
+      <c r="P14" s="13">
+        <f>AVERAGE(Q14:AB14)</f>
+        <v>777.91666666666663</v>
+      </c>
+      <c r="Q14" s="10">
         <v>927</v>
       </c>
-      <c r="Q14" s="4">
+      <c r="R14" s="4">
         <v>445</v>
       </c>
-      <c r="R14" s="4">
+      <c r="S14" s="4">
         <v>633</v>
       </c>
-      <c r="S14" s="6">
+      <c r="T14" s="6">
         <v>263</v>
       </c>
-      <c r="T14" s="4">
+      <c r="U14" s="4">
         <v>938</v>
       </c>
-      <c r="U14" s="4">
+      <c r="V14" s="4">
         <v>967</v>
       </c>
-      <c r="V14" s="1">
+      <c r="W14" s="1">
         <v>998</v>
       </c>
-      <c r="W14" s="1">
+      <c r="X14" s="1">
         <v>937</v>
       </c>
-      <c r="X14" s="1">
+      <c r="Y14" s="1">
         <v>866</v>
       </c>
-      <c r="Y14" s="1">
+      <c r="Z14" s="1">
         <v>633</v>
       </c>
-      <c r="Z14" s="1">
+      <c r="AA14" s="1">
         <v>929</v>
       </c>
-      <c r="AA14" s="6">
+      <c r="AB14" s="6">
         <v>799</v>
       </c>
-      <c r="AB14" s="1">
+      <c r="AC14" s="1">
         <v>962</v>
       </c>
-      <c r="AC14" s="1">
+      <c r="AD14" s="1">
         <v>972</v>
       </c>
-      <c r="AF14" s="1"/>
-      <c r="AG14" s="1">
+      <c r="AG14" s="1"/>
+      <c r="AH14" s="1">
         <f t="shared" si="0"/>
         <v>998</v>
       </c>
-      <c r="AH14" s="1"/>
+      <c r="AI14" s="1"/>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="4" t="s">
         <v>23</v>
@@ -2192,27 +2267,28 @@
       </c>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
-      <c r="P15" s="10"/>
-      <c r="Q15" s="4"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="10"/>
       <c r="R15" s="4"/>
-      <c r="S15" s="6"/>
-      <c r="T15" s="4"/>
+      <c r="S15" s="4"/>
+      <c r="T15" s="6"/>
       <c r="U15" s="4"/>
-      <c r="V15" s="1"/>
+      <c r="V15" s="4"/>
       <c r="W15" s="1"/>
       <c r="X15" s="1"/>
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
-      <c r="AA15" s="6"/>
-      <c r="AB15" s="1"/>
+      <c r="AA15" s="1"/>
+      <c r="AB15" s="6"/>
       <c r="AC15" s="1"/>
       <c r="AD15" s="1"/>
       <c r="AE15" s="1"/>
       <c r="AF15" s="1"/>
       <c r="AG15" s="1"/>
       <c r="AH15" s="1"/>
+      <c r="AI15" s="1"/>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="4" t="s">
         <v>24</v>
@@ -2252,27 +2328,28 @@
       </c>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
-      <c r="P16" s="10"/>
-      <c r="Q16" s="4"/>
+      <c r="P16" s="14"/>
+      <c r="Q16" s="10"/>
       <c r="R16" s="4"/>
-      <c r="S16" s="6"/>
-      <c r="T16" s="4"/>
+      <c r="S16" s="4"/>
+      <c r="T16" s="6"/>
       <c r="U16" s="4"/>
-      <c r="V16" s="1"/>
+      <c r="V16" s="4"/>
       <c r="W16" s="1"/>
       <c r="X16" s="1"/>
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
-      <c r="AA16" s="6"/>
-      <c r="AB16" s="1"/>
+      <c r="AA16" s="1"/>
+      <c r="AB16" s="6"/>
       <c r="AC16" s="1"/>
       <c r="AD16" s="1"/>
       <c r="AE16" s="1"/>
       <c r="AF16" s="1"/>
       <c r="AG16" s="1"/>
       <c r="AH16" s="1"/>
+      <c r="AI16" s="1"/>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -2287,17 +2364,13 @@
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
-      <c r="U17" s="1">
-        <f>AVERAGE(P2:AA2)</f>
-        <v>39.916666666666664</v>
-      </c>
-      <c r="V17" s="1"/>
+      <c r="U17" s="1"/>
       <c r="W17" s="1"/>
       <c r="X17" s="1"/>
       <c r="Y17" s="1"/>
@@ -2310,8 +2383,9 @@
       <c r="AF17" s="1"/>
       <c r="AG17" s="1"/>
       <c r="AH17" s="1"/>
+      <c r="AI17" s="1"/>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -2333,7 +2407,6 @@
       <c r="S18" s="1"/>
       <c r="T18" s="1"/>
       <c r="U18" s="1"/>
-      <c r="V18" s="1"/>
       <c r="W18" s="1"/>
       <c r="X18" s="1"/>
       <c r="Y18" s="1"/>
@@ -2346,8 +2419,9 @@
       <c r="AF18" s="1"/>
       <c r="AG18" s="1"/>
       <c r="AH18" s="1"/>
+      <c r="AI18" s="1"/>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -2369,7 +2443,6 @@
       <c r="S19" s="1"/>
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
-      <c r="V19" s="1"/>
       <c r="W19" s="1"/>
       <c r="X19" s="1"/>
       <c r="Y19" s="1"/>
@@ -2382,54 +2455,13 @@
       <c r="AF19" s="1"/>
       <c r="AG19" s="1"/>
       <c r="AH19" s="1"/>
+      <c r="AI19" s="1"/>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="U20" s="1">
-        <f t="shared" ref="U18:U31" si="1">AVERAGE(P5:AA5)</f>
-        <v>199.27272727272728</v>
-      </c>
+    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="V30" s="1"/>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="U21" s="1"/>
-    </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="U22" s="1"/>
-    </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="U23" s="1">
-        <f t="shared" si="1"/>
-        <v>14.583333333333334</v>
-      </c>
-    </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="U24" s="1"/>
-    </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="U25" s="1"/>
-    </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="U26" s="1">
-        <f t="shared" si="1"/>
-        <v>935.08333333333337</v>
-      </c>
-    </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="U27" s="1"/>
-    </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="U28" s="1"/>
-    </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="U29" s="1">
-        <f t="shared" si="1"/>
-        <v>777.91666666666663</v>
-      </c>
-    </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="U30" s="1"/>
-    </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="U31" s="1"/>
+    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="V31" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2">
@@ -3056,7 +3088,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P2:AA2">
+  <conditionalFormatting sqref="Q2:AB2">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -3068,7 +3100,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P5:AA5">
+  <conditionalFormatting sqref="Q5:AB5">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -3080,7 +3112,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P8:AA8">
+  <conditionalFormatting sqref="Q8:AB8">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -3092,7 +3124,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P11:AA11">
+  <conditionalFormatting sqref="Q11:AB11">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -3104,7 +3136,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P14:AA14">
+  <conditionalFormatting sqref="Q14:AB14">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>